<commit_message>
Fixed aspect ratio interpolation and root width
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05C6DFE-EC3D-424B-A21C-34730058FEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA4D993-A529-458F-AD71-0A2DFA29C42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
@@ -1162,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
   <dimension ref="A1:M213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
@@ -2170,11 +2170,11 @@
       </c>
       <c r="J54">
         <f>E57/E56</f>
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
       <c r="K54">
         <f>LOG10(J54)</f>
-        <v>-0.7269987279362623</v>
+        <v>-0.42596873227228116</v>
       </c>
       <c r="M54">
         <f>LOG10((E40+E41)/1000)</f>
@@ -2227,18 +2227,18 @@
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="15">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="G57">
         <v>48</v>
       </c>
       <c r="I57">
         <f>E52/E57</f>
-        <v>31.033333333333335</v>
+        <v>15.516666666666667</v>
       </c>
       <c r="J57">
         <f>(E40+E41)/1000/(E56*PI()/4*E57^2)</f>
-        <v>6.1893588980181518</v>
+        <v>1.5473397245045379</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
       </c>
       <c r="K59">
         <f>(K53-K54)/K54</f>
-        <v>-1.9187357001481846</v>
+        <v>-2.5680016741003988</v>
       </c>
       <c r="M59">
         <f>(M54-M53)/M54</f>
@@ -2326,6 +2326,18 @@
       </c>
       <c r="G62">
         <v>52</v>
+      </c>
+      <c r="J62">
+        <f>PI()/4*E53^2</f>
+        <v>3.1415926535897934E-2</v>
+      </c>
+      <c r="K62">
+        <f>0.907*J62/9</f>
+        <v>3.1660272631177143E-3</v>
+      </c>
+      <c r="L62">
+        <f>(4*K62/PI())^0.5</f>
+        <v>6.3491031737648682E-2</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3676,7 +3688,7 @@
   <dimension ref="A1:N211"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Resolved reproductive bug in integrator.py
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446BA301-7F0D-4B27-82DE-D803584E6CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68371F7A-3BAF-48AC-8242-934F62B3AD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="150">
   <si>
     <t>Parameter</t>
   </si>
@@ -615,6 +615,12 @@
   </si>
   <si>
     <t>elevation__above_WL</t>
+  </si>
+  <si>
+    <t>Dead biomass decay rate</t>
+  </si>
+  <si>
+    <t>biomass_decay_rate</t>
   </si>
 </sst>
 </file>
@@ -1160,15 +1166,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
-  <dimension ref="A1:M213"/>
+  <dimension ref="A1:M214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="41" style="23" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="23" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" style="15" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="24" customWidth="1"/>
@@ -1450,7 +1456,7 @@
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="15">
-        <v>180</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2270,250 +2276,247 @@
       <c r="E59" s="15">
         <v>0.01</v>
       </c>
-      <c r="K59">
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D60" s="19"/>
+      <c r="E60" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K60">
         <f>(K53-K54)/K54</f>
         <v>-2.5680016741003988</v>
       </c>
-      <c r="M59">
+      <c r="M60">
         <f>(M54-M53)/M54</f>
         <v>0.43665966442252035</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
+    <row r="61" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="8"/>
-      <c r="G60">
+      <c r="B61" s="5"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="8"/>
+      <c r="G61">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+    <row r="62" spans="1:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
         <v>125</v>
-      </c>
-      <c r="B61" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="15">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="G61">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
-        <v>126</v>
       </c>
       <c r="B62" s="19" t="s">
         <v>99</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D62" s="18"/>
       <c r="E62" s="15">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="G62">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D63" s="18"/>
+      <c r="E63" s="15">
         <v>0.5</v>
       </c>
-      <c r="G62">
+      <c r="G63">
         <v>52</v>
       </c>
-      <c r="J62">
+      <c r="J63">
         <f>PI()/4*E53^2</f>
         <v>3.1415926535897934E-2</v>
       </c>
-      <c r="K62">
-        <f>0.907*J62/9</f>
+      <c r="K63">
+        <f>0.907*J63/9</f>
         <v>3.1660272631177143E-3</v>
       </c>
-      <c r="L62">
-        <f>(4*K62/PI())^0.5</f>
+      <c r="L63">
+        <f>(4*K63/PI())^0.5</f>
         <v>6.3491031737648682E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B64" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C64" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D63" s="18"/>
-      <c r="E63" s="15">
+      <c r="D64" s="18"/>
+      <c r="E64" s="15">
         <f>20*0.2*0.69</f>
         <v>2.76</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>128</v>
       </c>
-      <c r="G63">
+      <c r="G64">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="5" t="s">
+    <row r="65" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="8"/>
-      <c r="G64">
+      <c r="B65" s="5"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="8"/>
+      <c r="G65">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="19" t="s">
+    <row r="66" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="s">
         <v>49</v>
-      </c>
-      <c r="B65" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D65" s="18"/>
-      <c r="E65" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="G65">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
-        <v>51</v>
       </c>
       <c r="B66" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D66" s="18"/>
       <c r="E66" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G66">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B67" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="18"/>
+      <c r="E67" s="15">
         <v>365</v>
       </c>
-      <c r="G66">
+      <c r="G67">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="5" t="s">
+    <row r="68" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="8" t="s">
+      <c r="B68" s="5"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G67">
+      <c r="G68">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
+    <row r="69" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="B68" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D68" s="18">
-        <v>1</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F68" t="s">
-        <v>107</v>
-      </c>
-      <c r="G68">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
-        <v>58</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D69" s="18">
         <v>1</v>
       </c>
-      <c r="E69" s="15">
-        <v>207</v>
+      <c r="E69" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="F69" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G69">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="D70" s="18">
         <v>1</v>
       </c>
-      <c r="E70" s="12" t="s">
-        <v>110</v>
+      <c r="E70" s="15">
+        <v>207</v>
       </c>
       <c r="F70" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="G70">
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B71" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D71" s="18">
         <v>1</v>
       </c>
-      <c r="E71">
-        <v>20</v>
-      </c>
-      <c r="G71">
-        <v>60</v>
+      <c r="E71" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F71" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
+      <c r="A72" s="19" t="s">
+        <v>59</v>
+      </c>
       <c r="B72" s="19" t="s">
         <v>100</v>
       </c>
@@ -2523,11 +2526,11 @@
       <c r="D72" s="18">
         <v>1</v>
       </c>
-      <c r="E72" s="15">
-        <v>30</v>
+      <c r="E72">
+        <v>20</v>
       </c>
       <c r="G72">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2542,10 +2545,10 @@
         <v>1</v>
       </c>
       <c r="E73" s="15">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="G73">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2560,10 +2563,10 @@
         <v>1</v>
       </c>
       <c r="E74" s="15">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G74">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2577,34 +2580,32 @@
       <c r="D75" s="18">
         <v>1</v>
       </c>
-      <c r="E75" s="15"/>
+      <c r="E75" s="15">
+        <v>100</v>
+      </c>
       <c r="G75">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
-        <v>114</v>
-      </c>
+      <c r="A76" s="19"/>
       <c r="B76" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D76" s="18">
         <v>1</v>
       </c>
-      <c r="E76" s="15">
-        <v>0</v>
-      </c>
+      <c r="E76" s="15"/>
       <c r="G76">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>100</v>
@@ -2616,15 +2617,15 @@
         <v>1</v>
       </c>
       <c r="E77" s="15">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G77">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>100</v>
@@ -2636,14 +2637,16 @@
         <v>1</v>
       </c>
       <c r="E78" s="15">
-        <v>0.67</v>
+        <v>0.01</v>
       </c>
       <c r="G78">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="19"/>
+      <c r="A79" s="19" t="s">
+        <v>116</v>
+      </c>
       <c r="B79" s="19" t="s">
         <v>100</v>
       </c>
@@ -2654,10 +2657,10 @@
         <v>1</v>
       </c>
       <c r="E79" s="15">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="G79">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2671,90 +2674,90 @@
       <c r="D80" s="18">
         <v>1</v>
       </c>
-      <c r="E80" s="15"/>
+      <c r="E80" s="15">
+        <v>1</v>
+      </c>
       <c r="G80">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
-        <v>61</v>
-      </c>
+      <c r="A81" s="19"/>
       <c r="B81" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D81" s="18">
-        <v>2</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E81" s="15"/>
       <c r="G81">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D82" s="18">
         <v>2</v>
       </c>
-      <c r="E82" s="15">
-        <v>365</v>
+      <c r="E82" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="G82">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="D83" s="18">
         <v>2</v>
       </c>
-      <c r="E83" s="12" t="s">
-        <v>110</v>
+      <c r="E83" s="15">
+        <v>365</v>
+      </c>
+      <c r="G83">
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D84" s="18">
         <v>2</v>
       </c>
-      <c r="E84" s="15">
-        <v>0</v>
-      </c>
-      <c r="G84">
-        <v>77</v>
+      <c r="E84" s="12" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="19"/>
+      <c r="A85" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="B85" s="19" t="s">
         <v>100</v>
       </c>
@@ -2765,10 +2768,10 @@
         <v>2</v>
       </c>
       <c r="E85" s="15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G85">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2783,10 +2786,10 @@
         <v>2</v>
       </c>
       <c r="E86" s="15">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G86">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2801,10 +2804,10 @@
         <v>2</v>
       </c>
       <c r="E87" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="G87">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2819,35 +2822,33 @@
         <v>2</v>
       </c>
       <c r="E88" s="15">
-        <v>1.69</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G88">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="19" t="s">
-        <v>64</v>
-      </c>
+      <c r="A89" s="19"/>
       <c r="B89" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D89" s="18">
         <v>2</v>
       </c>
       <c r="E89" s="15">
-        <v>0</v>
+        <v>1.69</v>
       </c>
       <c r="G89">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="B90" s="19" t="s">
         <v>100</v>
@@ -2862,12 +2863,12 @@
         <v>0</v>
       </c>
       <c r="G90">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>100</v>
@@ -2879,14 +2880,16 @@
         <v>2</v>
       </c>
       <c r="E91" s="15">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G91">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="19"/>
+      <c r="A92" s="19" t="s">
+        <v>116</v>
+      </c>
       <c r="B92" s="19" t="s">
         <v>100</v>
       </c>
@@ -2897,10 +2900,10 @@
         <v>2</v>
       </c>
       <c r="E92" s="15">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="G92">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -2918,14 +2921,26 @@
         <v>1</v>
       </c>
       <c r="G93">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="19"/>
+      <c r="B94" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D94" s="18">
+        <v>2</v>
+      </c>
+      <c r="E94" s="15">
+        <v>1</v>
+      </c>
+      <c r="G94">
         <v>86</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="20"/>
-      <c r="B94" s="20"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="22"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="20"/>
@@ -3583,6 +3598,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="20"/>
+      <c r="B204" s="20"/>
       <c r="C204" s="21"/>
       <c r="D204" s="22"/>
     </row>
@@ -3630,6 +3646,11 @@
       <c r="A213" s="20"/>
       <c r="C213" s="21"/>
       <c r="D213" s="22"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="20"/>
+      <c r="C214" s="21"/>
+      <c r="D214" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3649,10 +3670,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{FCAB33B4-E22D-416A-9EE8-1B6629F4B7A9}">
       <formula1>"angiosperm, gymnosperm"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E66" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E67" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E30 E67 E62 E64:E65" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E30 E68 E63 E65:E66" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -3678,7 +3699,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{793E17DF-C558-4DAF-B608-9E20297CD619}">
       <formula1>"evergreen, deciduous"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E70 E83" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E71 E84" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3689,10 +3710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
-  <dimension ref="A1:N211"/>
+  <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3967,59 +3988,56 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>24</v>
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="15">
+      <c r="D17" s="11"/>
+      <c r="E17" s="15">
         <v>273</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="8"/>
-      <c r="G17">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="8"/>
+      <c r="G18">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+    <row r="19" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" s="15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G18">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
       <c r="B19" s="9" t="s">
         <v>92</v>
       </c>
@@ -4027,13 +4045,13 @@
         <v>67</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G19">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -4045,13 +4063,13 @@
         <v>67</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E20" s="15">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G20">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -4063,13 +4081,13 @@
         <v>67</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E21" s="15">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="G21">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4081,37 +4099,37 @@
         <v>67</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E22" s="15">
         <v>0.01</v>
       </c>
       <c r="G22">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>27</v>
-      </c>
+      <c r="A23" s="28"/>
       <c r="B23" s="9" t="s">
         <v>92</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E23" s="15">
-        <v>1.444</v>
+        <v>0.01</v>
       </c>
       <c r="G23">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+      <c r="A24" s="28" t="s">
+        <v>27</v>
+      </c>
       <c r="B24" s="9" t="s">
         <v>92</v>
       </c>
@@ -4119,13 +4137,13 @@
         <v>28</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" s="15">
-        <v>1.5129999999999999</v>
+        <v>1.444</v>
       </c>
       <c r="G24">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4137,13 +4155,13 @@
         <v>28</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="15">
-        <v>1.4630000000000001</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="G25">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -4155,13 +4173,13 @@
         <v>28</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E26" s="15">
-        <v>1.415</v>
+        <v>1.4630000000000001</v>
       </c>
       <c r="G26">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4173,98 +4191,94 @@
         <v>28</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E27" s="15">
-        <v>1.4139999999999999</v>
+        <v>1.415</v>
       </c>
       <c r="G27">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="A28" s="28"/>
       <c r="B28" s="9" t="s">
         <v>92</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="11"/>
+        <v>28</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>96</v>
+      </c>
       <c r="E28" s="15">
-        <v>0.48</v>
+        <v>1.4139999999999999</v>
       </c>
       <c r="G28">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="32.25" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>92</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="15">
-        <v>100</v>
-      </c>
-      <c r="F29" t="s">
-        <v>66</v>
+        <v>0.48</v>
       </c>
       <c r="G29">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>92</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="15">
-        <v>0.05</v>
+        <v>100</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
       </c>
       <c r="G30">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="31" t="s">
-        <v>103</v>
+        <v>34</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="15">
+        <v>0.05</v>
       </c>
       <c r="G31">
-        <v>27</v>
-      </c>
-      <c r="H31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="B32" s="9" t="s">
         <v>92</v>
       </c>
@@ -4272,12 +4286,17 @@
         <v>101</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E32" s="15"/>
-      <c r="F32" s="31"/>
+      <c r="F32" s="31" t="s">
+        <v>103</v>
+      </c>
       <c r="G32">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="H32" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -4289,12 +4308,12 @@
         <v>101</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="31"/>
       <c r="G33">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -4303,15 +4322,15 @@
         <v>92</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="31"/>
       <c r="G34">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -4323,12 +4342,12 @@
         <v>102</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E35" s="15"/>
       <c r="F35" s="31"/>
       <c r="G35">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -4340,36 +4359,35 @@
         <v>102</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E36" s="15"/>
       <c r="F36" s="31"/>
       <c r="G36">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
-        <v>41</v>
-      </c>
+      <c r="A37" s="29"/>
       <c r="B37" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="15">
-        <v>0.01</v>
-      </c>
+      <c r="C37" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="31"/>
       <c r="G37">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A38" s="30" t="s">
+        <v>41</v>
+      </c>
       <c r="B38" s="9" t="s">
         <v>92</v>
       </c>
@@ -4377,14 +4395,13 @@
         <v>42</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E38" s="27">
-        <f>E39/0.27*0.2</f>
-        <v>2.2222222222222223E-2</v>
+        <v>104</v>
+      </c>
+      <c r="E38" s="15">
+        <v>0.01</v>
       </c>
       <c r="G38">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -4396,13 +4413,14 @@
         <v>42</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E39" s="15">
-        <v>0.03</v>
+        <v>105</v>
+      </c>
+      <c r="E39" s="27">
+        <f>E40/0.27*0.2</f>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="G39">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -4414,13 +4432,13 @@
         <v>42</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E40" s="15">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="G40">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -4432,37 +4450,37 @@
         <v>42</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E41" s="15">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G41">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
-        <v>78</v>
-      </c>
+      <c r="A42" s="30"/>
       <c r="B42" s="9" t="s">
         <v>92</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E42" s="15">
-        <v>4.3</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="30" t="s">
+        <v>78</v>
+      </c>
       <c r="B43" s="9" t="s">
         <v>92</v>
       </c>
@@ -4470,29 +4488,13 @@
         <v>79</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E43" s="15">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="G43">
-        <v>39</v>
-      </c>
-      <c r="J43">
-        <f>E43+E44</f>
-        <v>9.6</v>
-      </c>
-      <c r="K43">
-        <f>LOG10(J43/1000)</f>
-        <v>-2.0177287669604316</v>
-      </c>
-      <c r="M43">
-        <f>E50/E51</f>
-        <v>2.5</v>
-      </c>
-      <c r="N43">
-        <f>LOG10(M43)</f>
-        <v>0.3979400086720376</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -4504,29 +4506,29 @@
         <v>79</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E44" s="15">
-        <v>5.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G44">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J44">
-        <f>(E38+E39)/E54*E50</f>
-        <v>0.52222222222222237</v>
+        <f>E44+E45</f>
+        <v>9.6</v>
       </c>
       <c r="K44">
         <f>LOG10(J44/1000)</f>
-        <v>-3.2821446515036072</v>
+        <v>-2.0177287669604316</v>
       </c>
       <c r="M44">
-        <f>E50/E55</f>
-        <v>138.2930051648863</v>
+        <f>E51/E52</f>
+        <v>2.5</v>
       </c>
       <c r="N44">
         <f>LOG10(M44)</f>
-        <v>2.1408002141287135</v>
+        <v>0.3979400086720376</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -4538,13 +4540,29 @@
         <v>79</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E45" s="15">
-        <v>1</v>
+        <v>5.5</v>
       </c>
       <c r="G45">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="J45">
+        <f>(E39+E40)/E55*E51</f>
+        <v>0.52222222222222237</v>
+      </c>
+      <c r="K45">
+        <f>LOG10(J45/1000)</f>
+        <v>-3.2821446515036072</v>
+      </c>
+      <c r="M45">
+        <f>E51/E56</f>
+        <v>138.2930051648863</v>
+      </c>
+      <c r="N45">
+        <f>LOG10(M45)</f>
+        <v>2.1408002141287135</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -4556,445 +4574,450 @@
         <v>79</v>
       </c>
       <c r="D46" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" s="15">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="30"/>
+      <c r="B47" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E47" s="15">
         <v>4</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="8"/>
-      <c r="G47">
+      <c r="B48" s="5"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="8"/>
+      <c r="G48">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+    <row r="49" spans="1:13" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="15">
-        <v>18</v>
-      </c>
-      <c r="G48">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
-        <v>46</v>
       </c>
       <c r="B49" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D49" s="18"/>
       <c r="E49" s="15">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G49">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="B50" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>131</v>
+        <v>47</v>
       </c>
       <c r="D50" s="18"/>
       <c r="E50" s="15">
-        <v>0.75</v>
+        <v>10</v>
       </c>
       <c r="G50">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="D51" s="18"/>
       <c r="E51" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="J51">
-        <f>PI()/4*E51^2*E50</f>
-        <v>5.3014376029327764E-2</v>
-      </c>
-      <c r="K51">
-        <f>J43/1000/J51</f>
-        <v>0.18108295747344533</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="G51">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D52" s="18"/>
       <c r="E52" s="15">
-        <v>0.33</v>
-      </c>
-      <c r="I52">
-        <f>E50/E55</f>
-        <v>138.2930051648863</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+      <c r="J52">
+        <f>PI()/4*E52^2*E51</f>
+        <v>5.3014376029327764E-2</v>
+      </c>
+      <c r="K52">
+        <f>J44/1000/J52</f>
+        <v>0.18108295747344533</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B53" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D53" s="18"/>
       <c r="E53" s="15">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="I53">
-        <f>E50/E51</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <f>E51/E56</f>
+        <v>138.2930051648863</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B54" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D54" s="18"/>
       <c r="E54" s="15">
-        <f>E50/10</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.35</v>
+      </c>
+      <c r="I54">
+        <f>E51/E52</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B55" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C55" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" s="18"/>
+      <c r="E55" s="15">
+        <f>E51/10</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="D55" s="18"/>
-      <c r="E55" s="27">
+      <c r="D56" s="18"/>
+      <c r="E56" s="27">
         <f>SQRT(0.231/100/100*4/PI())</f>
         <v>5.423267786434878E-3</v>
       </c>
-      <c r="G55">
+      <c r="G56">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
         <v>135</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="18"/>
-      <c r="E56" s="15">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
-        <v>137</v>
       </c>
       <c r="B57" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="18"/>
+      <c r="E58" s="15">
         <v>0.01</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D59" s="19"/>
+      <c r="E59" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K59" t="e">
+        <f>(K52-K53)/K53</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M59" t="e">
+        <f>(M53-M52)/M53</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="8"/>
-      <c r="G58">
+      <c r="B60" s="5"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="8"/>
+      <c r="G60">
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+    <row r="61" spans="1:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="19" t="s">
         <v>125</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D59" s="18"/>
-      <c r="E59" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="G59">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B60" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G60">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
-        <v>127</v>
       </c>
       <c r="B61" s="19" t="s">
         <v>99</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="D61" s="18"/>
       <c r="E61" s="15">
-        <v>1.2</v>
-      </c>
-      <c r="F61" t="s">
-        <v>128</v>
+        <v>0.4</v>
       </c>
       <c r="G61">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="8"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D62" s="18"/>
+      <c r="E62" s="15">
+        <v>0.5</v>
+      </c>
       <c r="G62">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="D63" s="18"/>
       <c r="E63" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="F63" t="s">
+        <v>128</v>
+      </c>
+      <c r="G63">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="8"/>
+      <c r="G64">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" s="18"/>
+      <c r="E65" s="15">
         <v>0.01</v>
       </c>
-      <c r="G63">
+      <c r="G65">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B66" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="C66" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D64" s="18"/>
-      <c r="E64" s="15">
+      <c r="D66" s="18"/>
+      <c r="E66" s="15">
         <v>365</v>
       </c>
-      <c r="G64">
+      <c r="G66">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="5" t="s">
+    <row r="67" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="8" t="s">
+      <c r="B67" s="5"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G65">
+      <c r="G67">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+    <row r="68" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="B66" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D66" s="18">
-        <v>1</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F66" t="s">
-        <v>57</v>
-      </c>
-      <c r="G66">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B67" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D67" s="18">
-        <v>1</v>
-      </c>
-      <c r="E67" s="15">
-        <v>207</v>
-      </c>
-      <c r="G67">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="D68" s="18">
         <v>1</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="F68" t="s">
-        <v>113</v>
+        <v>57</v>
+      </c>
+      <c r="G68">
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D69" s="18">
         <v>1</v>
       </c>
       <c r="E69" s="15">
-        <v>30</v>
+        <v>207</v>
       </c>
       <c r="G69">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
+      <c r="A70" s="19" t="s">
+        <v>108</v>
+      </c>
       <c r="B70" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D70" s="18">
         <v>1</v>
       </c>
-      <c r="E70" s="15">
-        <v>40</v>
-      </c>
-      <c r="G70">
-        <v>61</v>
+      <c r="E70" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F70" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="19"/>
+      <c r="A71" s="19" t="s">
+        <v>59</v>
+      </c>
       <c r="B71" s="19" t="s">
         <v>100</v>
       </c>
@@ -5005,10 +5028,10 @@
         <v>1</v>
       </c>
       <c r="E71" s="15">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G71">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -5023,10 +5046,10 @@
         <v>1</v>
       </c>
       <c r="E72" s="15">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="G72">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -5040,29 +5063,29 @@
       <c r="D73" s="18">
         <v>1</v>
       </c>
-      <c r="E73" s="15"/>
+      <c r="E73" s="15">
+        <v>50</v>
+      </c>
       <c r="G73">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="19" t="s">
-        <v>60</v>
-      </c>
+      <c r="A74" s="19"/>
       <c r="B74" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D74" s="18">
         <v>1</v>
       </c>
       <c r="E74" s="15">
-        <v>0.01</v>
+        <v>55</v>
       </c>
       <c r="G74">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -5071,20 +5094,20 @@
         <v>100</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D75" s="18">
         <v>1</v>
       </c>
-      <c r="E75" s="15">
-        <v>0.25</v>
-      </c>
+      <c r="E75" s="15"/>
       <c r="G75">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="19"/>
+      <c r="A76" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="B76" s="19" t="s">
         <v>100</v>
       </c>
@@ -5095,10 +5118,10 @@
         <v>1</v>
       </c>
       <c r="E76" s="15">
-        <v>0.67</v>
+        <v>0.01</v>
       </c>
       <c r="G76">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -5113,10 +5136,10 @@
         <v>1</v>
       </c>
       <c r="E77" s="15">
-        <v>0.9</v>
+        <v>0.25</v>
       </c>
       <c r="G77">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -5130,111 +5153,111 @@
       <c r="D78" s="18">
         <v>1</v>
       </c>
-      <c r="E78" s="15"/>
+      <c r="E78" s="15">
+        <v>0.67</v>
+      </c>
       <c r="G78">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
-        <v>61</v>
-      </c>
+      <c r="A79" s="19"/>
       <c r="B79" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D79" s="18">
-        <v>2</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>147</v>
+        <v>1</v>
+      </c>
+      <c r="E79" s="15">
+        <v>0.9</v>
       </c>
       <c r="G79">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="A80" s="19"/>
       <c r="B80" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="D80" s="18">
-        <v>2</v>
-      </c>
-      <c r="E80" s="15">
-        <v>365</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E80" s="15"/>
       <c r="G80">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="19" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="D81" s="18">
         <v>2</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F81" t="s">
-        <v>113</v>
+        <v>147</v>
+      </c>
+      <c r="G81">
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D82" s="18">
         <v>2</v>
       </c>
       <c r="E82" s="15">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G82">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="19"/>
+      <c r="A83" s="19" t="s">
+        <v>111</v>
+      </c>
       <c r="B83" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D83" s="18">
         <v>2</v>
       </c>
-      <c r="E83" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G83">
-        <v>78</v>
+      <c r="E83" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F83" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="19"/>
+      <c r="A84" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="B84" s="19" t="s">
         <v>100</v>
       </c>
@@ -5245,10 +5268,10 @@
         <v>2</v>
       </c>
       <c r="E84" s="15">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G84">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -5263,10 +5286,10 @@
         <v>2</v>
       </c>
       <c r="E85" s="15">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="G85">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -5281,30 +5304,28 @@
         <v>2</v>
       </c>
       <c r="E86" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="G86">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="19" t="s">
-        <v>64</v>
-      </c>
+      <c r="A87" s="19"/>
       <c r="B87" s="19" t="s">
         <v>100</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D87" s="18">
         <v>2</v>
       </c>
       <c r="E87" s="15">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="G87">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -5313,20 +5334,22 @@
         <v>100</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D88" s="18">
         <v>2</v>
       </c>
       <c r="E88" s="15">
-        <v>0</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G88">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="19"/>
+      <c r="A89" s="19" t="s">
+        <v>64</v>
+      </c>
       <c r="B89" s="19" t="s">
         <v>100</v>
       </c>
@@ -5337,10 +5360,10 @@
         <v>2</v>
       </c>
       <c r="E89" s="15">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G89">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -5355,10 +5378,10 @@
         <v>2</v>
       </c>
       <c r="E90" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -5373,23 +5396,47 @@
         <v>2</v>
       </c>
       <c r="E91" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="G91">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="19"/>
+      <c r="B92" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D92" s="18">
+        <v>2</v>
+      </c>
+      <c r="E92" s="15">
         <v>1</v>
       </c>
-      <c r="G91">
+      <c r="G92">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="19"/>
+      <c r="B93" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C93" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D93" s="18">
+        <v>2</v>
+      </c>
+      <c r="E93" s="15">
+        <v>1</v>
+      </c>
+      <c r="G93">
         <v>86</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="20"/>
-      <c r="B92" s="20"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="22"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="20"/>
-      <c r="B93" s="20"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="22"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
@@ -6099,34 +6146,46 @@
       <c r="C211" s="21"/>
       <c r="D211" s="22"/>
     </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="20"/>
+      <c r="B212" s="20"/>
+      <c r="C212" s="21"/>
+      <c r="D212" s="22"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="20"/>
+      <c r="B213" s="20"/>
+      <c r="C213" s="21"/>
+      <c r="D213" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="F31:F36"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="F32:F37"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A38:A42"/>
   </mergeCells>
   <dataValidations count="14">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{76366DFC-F994-4B24-8F58-3C475A37D29A}">
       <formula1>"annual, perennial"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12 E17" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12 E18" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
       <formula1>"Annual, Herbaceous perennial, Woody perennial"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11" xr:uid="{BF09F0A8-DEDC-4564-B7AE-B6347D314DF5}">
       <formula1>"C3, C4, CAM"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E16" xr:uid="{2135F1C0-D38D-4F5D-8EF7-81232862BF29}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E17" xr:uid="{2135F1C0-D38D-4F5D-8EF7-81232862BF29}">
       <formula1>1</formula1>
       <formula2>366</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28 E65 E60 E62:E63" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E29 E67 E62 E64:E65" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E64" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E66" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{9966BE53-3AF7-47D9-9DC3-79C6924CF42E}">
@@ -6150,7 +6209,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{82D88EBD-3D9A-4158-A9B3-F883994282C6}">
       <formula1>"climbing,columnar,conical,decumbent,erect,irregular,oval,prostrate,rounded,semi_erect,vase"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E68 E81" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E70 E83" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added SLA to morph_params
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F99DCC9-6808-4246-91EB-1902BB630035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF666285-C08E-47E4-AF22-5BF476D6D893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="-38400" yWindow="-16190" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="159">
   <si>
     <t>Parameter</t>
   </si>
@@ -636,6 +636,43 @@
   </si>
   <si>
     <t>incremental_nsc</t>
+  </si>
+  <si>
+    <t>Peak biomass (day-of-year)</t>
+  </si>
+  <si>
+    <t>peak_biomass</t>
+  </si>
+  <si>
+    <r>
+      <t>Specific leaf area (m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/g)</t>
+    </r>
+  </si>
+  <si>
+    <t>sp_leaf_area</t>
   </si>
 </sst>
 </file>
@@ -1187,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
-  <dimension ref="A1:M225"/>
+  <dimension ref="A1:M227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:A59"/>
+    <sheetView topLeftCell="A28" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:XFD72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,107 +1466,104 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>78</v>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="18"/>
+      <c r="C14" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="11"/>
       <c r="E14" s="15">
-        <v>140</v>
-      </c>
-      <c r="G14">
-        <v>50</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>137</v>
+        <v>78</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="15">
-        <v>226</v>
+        <v>140</v>
+      </c>
+      <c r="G15">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>23</v>
+      <c r="A16" s="19" t="s">
+        <v>137</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="15">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>139</v>
+        <v>23</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="15">
+      <c r="D18" s="11"/>
+      <c r="E18" s="15">
         <v>1000</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="8"/>
-      <c r="G18">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="8"/>
+      <c r="G19">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+    <row r="20" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
       <c r="B20" s="9" t="s">
         <v>87</v>
       </c>
@@ -1537,13 +1571,13 @@
         <v>65</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G20">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1555,17 +1589,17 @@
         <v>65</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E21" s="15">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G21">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="9" t="s">
         <v>87</v>
       </c>
@@ -1573,37 +1607,37 @@
         <v>65</v>
       </c>
       <c r="D22" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="G22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E23" s="15">
         <v>0.01</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="15">
-        <v>1.444</v>
-      </c>
-      <c r="G23">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
       <c r="B24" s="9" t="s">
         <v>87</v>
       </c>
@@ -1611,13 +1645,13 @@
         <v>27</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E24" s="15">
-        <v>1.5129999999999999</v>
+        <v>1.444</v>
       </c>
       <c r="G24">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1629,13 +1663,13 @@
         <v>27</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E25" s="15">
-        <v>1.4630000000000001</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="G25">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1647,98 +1681,94 @@
         <v>27</v>
       </c>
       <c r="D26" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="15">
+        <v>1.4630000000000001</v>
+      </c>
+      <c r="G26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
+      <c r="B27" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E27" s="15">
         <v>1.4139999999999999</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="10" t="s">
+      <c r="B28" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="15">
-        <v>0.51</v>
-      </c>
-      <c r="G27">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="15">
-        <v>100</v>
-      </c>
-      <c r="F28" t="s">
-        <v>64</v>
+        <v>0.51</v>
       </c>
       <c r="G28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="15">
+        <v>100</v>
+      </c>
+      <c r="F29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="15">
         <v>3.7199999999999997E-2</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30">
-        <v>27</v>
-      </c>
-      <c r="H30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
       <c r="B31" s="9" t="s">
         <v>87</v>
       </c>
@@ -1746,11 +1776,17 @@
         <v>95</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E31" s="15"/>
+      <c r="F31" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="G31">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="H31" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1762,11 +1798,11 @@
         <v>95</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32" s="15"/>
       <c r="G32">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -1775,14 +1811,14 @@
         <v>87</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E33" s="15"/>
       <c r="G33">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -1794,11 +1830,11 @@
         <v>96</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E34" s="15"/>
       <c r="G34">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -1810,51 +1846,33 @@
         <v>96</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35" s="15"/>
       <c r="G35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="30"/>
+      <c r="B36" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="G36">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="G36">
-        <v>33</v>
-      </c>
-      <c r="J36">
-        <f>E38+E37</f>
-        <v>0.7</v>
-      </c>
-      <c r="K36">
-        <f>LOG10(J36/1000)</f>
-        <v>-3.1549019599857431</v>
-      </c>
-      <c r="L36">
-        <f>J36/E67*E63</f>
-        <v>4.0731250000000001</v>
-      </c>
-      <c r="M36">
-        <f>LOG10(L36/1000)</f>
-        <v>-2.3900722616603254</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
       <c r="B37" s="9" t="s">
         <v>87</v>
       </c>
@@ -1862,13 +1880,29 @@
         <v>41</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E37" s="15">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="G37">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="J37">
+        <f>E39+E38</f>
+        <v>0.7</v>
+      </c>
+      <c r="K37">
+        <f>LOG10(J37/1000)</f>
+        <v>-3.1549019599857431</v>
+      </c>
+      <c r="L37">
+        <f>J37/E68*E64</f>
+        <v>4.0731250000000001</v>
+      </c>
+      <c r="M37">
+        <f>LOG10(L37/1000)</f>
+        <v>-2.3900722616603254</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -1880,17 +1914,17 @@
         <v>41</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E38" s="15">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G38">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="9" t="s">
         <v>87</v>
       </c>
@@ -1898,37 +1932,37 @@
         <v>41</v>
       </c>
       <c r="D39" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G39">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
+      <c r="B40" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E40" s="15">
         <v>0</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="15">
-        <v>10.9</v>
-      </c>
-      <c r="G40">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
       <c r="B41" s="9" t="s">
         <v>87</v>
       </c>
@@ -1936,21 +1970,13 @@
         <v>75</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E41" s="15">
-        <v>6.68</v>
+        <v>10.9</v>
       </c>
       <c r="G41">
-        <v>39</v>
-      </c>
-      <c r="J41">
-        <f>E42+E41</f>
-        <v>16.7</v>
-      </c>
-      <c r="K41">
-        <f>LOG10(J41)</f>
-        <v>1.2227164711475833</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -1962,13 +1988,21 @@
         <v>75</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E42" s="15">
-        <v>10.02</v>
+        <v>6.68</v>
       </c>
       <c r="G42">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="J42">
+        <f>E43+E42</f>
+        <v>16.7</v>
+      </c>
+      <c r="K42">
+        <f>LOG10(J42)</f>
+        <v>1.2227164711475833</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -1980,35 +2014,37 @@
         <v>75</v>
       </c>
       <c r="D43" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="15">
+        <v>10.02</v>
+      </c>
+      <c r="G43">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="28"/>
+      <c r="B44" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E44" s="15">
         <v>18</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="16" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
       <c r="B45" s="9" t="s">
         <v>87</v>
       </c>
@@ -2016,7 +2052,7 @@
         <v>147</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E45" s="15"/>
       <c r="F45" s="16" t="s">
@@ -2032,7 +2068,7 @@
         <v>147</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="16" t="s">
@@ -2048,7 +2084,7 @@
         <v>147</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="16" t="s">
@@ -2056,41 +2092,25 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
-        <v>151</v>
-      </c>
+      <c r="A48" s="28"/>
       <c r="B48" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E48" s="15"/>
       <c r="F48" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="I48">
-        <f>E63/E64</f>
-        <v>4.6550000000000002</v>
-      </c>
-      <c r="J48">
-        <f>E63/E64</f>
-        <v>4.6550000000000002</v>
-      </c>
-      <c r="K48">
-        <f>LOG10(J48)</f>
-        <v>0.66791968531736146</v>
-      </c>
-      <c r="M48">
-        <f>LOG10((E41+E42)/1000)</f>
-        <v>-1.7772835288524167</v>
-      </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+      <c r="A49" s="28" t="s">
+        <v>151</v>
+      </c>
       <c r="B49" s="9" t="s">
         <v>87</v>
       </c>
@@ -2098,23 +2118,27 @@
         <v>145</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E49" s="15"/>
       <c r="F49" s="16" t="s">
         <v>149</v>
       </c>
+      <c r="I49">
+        <f>E64/E65</f>
+        <v>4.6550000000000002</v>
+      </c>
       <c r="J49">
-        <f>E68/E67</f>
-        <v>0.375</v>
+        <f>E64/E65</f>
+        <v>4.6550000000000002</v>
       </c>
       <c r="K49">
         <f>LOG10(J49)</f>
-        <v>-0.42596873227228116</v>
+        <v>0.66791968531736146</v>
       </c>
       <c r="M49">
-        <f>LOG10((E37+E38)/1000)</f>
-        <v>-3.1549019599857431</v>
+        <f>LOG10((E42+E43)/1000)</f>
+        <v>-1.7772835288524167</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -2126,12 +2150,24 @@
         <v>145</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E50" s="15"/>
       <c r="F50" s="16" t="s">
         <v>149</v>
       </c>
+      <c r="J50">
+        <f>E69/E68</f>
+        <v>0.375</v>
+      </c>
+      <c r="K50">
+        <f>LOG10(J50)</f>
+        <v>-0.42596873227228116</v>
+      </c>
+      <c r="M50">
+        <f>LOG10((E38+E39)/1000)</f>
+        <v>-3.1549019599857431</v>
+      </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="28"/>
@@ -2142,45 +2178,37 @@
         <v>145</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="J51">
-        <f>(E41+E42)/1000/(E63*PI()/4*E64^2)</f>
-        <v>0.57097476898703581</v>
-      </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
-        <v>152</v>
-      </c>
+      <c r="A52" s="28"/>
       <c r="B52" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E52" s="15"/>
       <c r="F52" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="I52">
-        <f>E63/E68</f>
-        <v>15.516666666666667</v>
-      </c>
       <c r="J52">
-        <f>(E37+E38)/1000/(E67*PI()/4*E68^2)</f>
-        <v>1.5473397245045379</v>
+        <f>(E42+E43)/1000/(E64*PI()/4*E65^2)</f>
+        <v>0.57097476898703581</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
+      <c r="A53" s="28" t="s">
+        <v>152</v>
+      </c>
       <c r="B53" s="9" t="s">
         <v>87</v>
       </c>
@@ -2188,12 +2216,20 @@
         <v>148</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E53" s="15"/>
       <c r="F53" s="16" t="s">
         <v>149</v>
       </c>
+      <c r="I53">
+        <f>E64/E69</f>
+        <v>15.516666666666667</v>
+      </c>
+      <c r="J53">
+        <f>(E38+E39)/1000/(E68*PI()/4*E69^2)</f>
+        <v>1.5473397245045379</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="28"/>
@@ -2204,7 +2240,7 @@
         <v>148</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E54" s="15"/>
       <c r="F54" s="16" t="s">
@@ -2220,41 +2256,41 @@
         <v>148</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="K55">
-        <f>(K48-K49)/K49</f>
-        <v>-2.5680016741003988</v>
-      </c>
-      <c r="M55">
-        <f>(M49-M48)/M49</f>
-        <v>0.43665966442252035</v>
-      </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
-        <v>153</v>
-      </c>
+      <c r="A56" s="28"/>
       <c r="B56" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="16" t="s">
         <v>149</v>
       </c>
+      <c r="K56">
+        <f>(K49-K50)/K50</f>
+        <v>-2.5680016741003988</v>
+      </c>
+      <c r="M56">
+        <f>(M50-M49)/M50</f>
+        <v>0.43665966442252035</v>
+      </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
+      <c r="A57" s="28" t="s">
+        <v>153</v>
+      </c>
       <c r="B57" s="9" t="s">
         <v>87</v>
       </c>
@@ -2262,7 +2298,7 @@
         <v>154</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E57" s="15"/>
       <c r="F57" s="16" t="s">
@@ -2278,7 +2314,7 @@
         <v>154</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E58" s="15"/>
       <c r="F58" s="16" t="s">
@@ -2294,447 +2330,442 @@
         <v>154</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E59" s="15"/>
       <c r="F59" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="28"/>
+      <c r="B60" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E60" s="15"/>
+      <c r="F60" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="8"/>
-    </row>
-    <row r="61" spans="1:13" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="B61" s="5"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:13" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
         <v>43</v>
-      </c>
-      <c r="B61" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="15">
-        <v>100</v>
-      </c>
-      <c r="G61">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="B62" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D62" s="18"/>
       <c r="E62" s="15">
-        <v>9</v>
+        <v>100</v>
+      </c>
+      <c r="G62">
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B63" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="D63" s="18"/>
       <c r="E63" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" s="18"/>
+      <c r="E64" s="15">
         <f>0.91+3*0.007</f>
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="B64" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D64" s="18"/>
-      <c r="E64" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="G64">
-        <v>48</v>
-      </c>
-    </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B65" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="15">
-        <v>1.45</v>
+        <v>0.2</v>
+      </c>
+      <c r="G65">
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B66" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D66" s="18"/>
       <c r="E66" s="15">
-        <v>0.5</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B67" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D67" s="18"/>
       <c r="E67" s="15">
-        <v>0.16</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="15">
-        <v>0.06</v>
-      </c>
-      <c r="G68">
-        <v>49</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D69" s="18"/>
       <c r="E69" s="15">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="G69">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D70" s="18"/>
       <c r="E70" s="15">
         <v>0.01</v>
       </c>
       <c r="G70">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B71" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="18"/>
+      <c r="E71" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G71">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A72" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="15">
+        <v>6.6309999999999997E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="D71" s="19"/>
-      <c r="E71" s="15">
+      <c r="D73" s="19"/>
+      <c r="E73" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" t="s">
         <v>122</v>
       </c>
-      <c r="G71">
+      <c r="G73">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="5" t="s">
+    <row r="74" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="8"/>
-      <c r="G72">
+      <c r="B74" s="5"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="8"/>
+      <c r="G74">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+    <row r="75" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="B73" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D73" s="18"/>
-      <c r="E73" s="15">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="G73">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B74" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G74">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="19" t="s">
-        <v>121</v>
       </c>
       <c r="B75" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="D75" s="18"/>
       <c r="E75" s="15">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="G75">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" s="18"/>
+      <c r="E76" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G76">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D77" s="18"/>
+      <c r="E77" s="15">
         <f>20*0.2*0.69</f>
         <v>2.76</v>
       </c>
-      <c r="F75" s="8" t="s">
+      <c r="F77" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G75">
+      <c r="G77">
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
+    <row r="78" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="6"/>
-      <c r="F76" t="s">
+      <c r="B78" s="5"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="6"/>
+      <c r="F78" t="s">
         <v>101</v>
       </c>
-      <c r="G76">
+      <c r="G78">
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
+    <row r="79" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B77" s="19" t="s">
+      <c r="B79" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="C79" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D77" s="18"/>
-      <c r="E77" s="15">
+      <c r="D79" s="18"/>
+      <c r="E79" s="15">
         <v>0.01</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F79" t="s">
         <v>106</v>
       </c>
-      <c r="G77">
+      <c r="G79">
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="B80" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="C80" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D78" s="18"/>
-      <c r="E78" s="15">
+      <c r="D80" s="18"/>
+      <c r="E80" s="15">
         <v>365</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F80" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="5" t="s">
+    <row r="81" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="6"/>
-      <c r="G79">
+      <c r="B81" s="5"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="6"/>
+      <c r="G81">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
+    <row r="82" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C80" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D80" s="18">
-        <v>1</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G80">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D81" s="18">
-        <v>1</v>
-      </c>
-      <c r="E81" s="15">
-        <v>207</v>
-      </c>
-      <c r="G81">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
-        <v>102</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D82" s="18">
         <v>1</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="G82">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D83" s="18">
         <v>1</v>
       </c>
-      <c r="E83">
-        <v>20</v>
+      <c r="E83" s="15">
+        <v>207</v>
       </c>
       <c r="G83">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="19"/>
+      <c r="A84" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="B84" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D84" s="18">
         <v>1</v>
       </c>
-      <c r="E84" s="15">
-        <v>30</v>
+      <c r="E84" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="G84">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="19"/>
+      <c r="A85" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="B85" s="19" t="s">
         <v>94</v>
       </c>
@@ -2744,11 +2775,11 @@
       <c r="D85" s="18">
         <v>1</v>
       </c>
-      <c r="E85" s="15">
-        <v>70</v>
+      <c r="E85">
+        <v>20</v>
       </c>
       <c r="G85">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2763,10 +2794,10 @@
         <v>1</v>
       </c>
       <c r="E86" s="15">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="G86">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2780,54 +2811,50 @@
       <c r="D87" s="18">
         <v>1</v>
       </c>
-      <c r="E87" s="15"/>
+      <c r="E87" s="15">
+        <v>70</v>
+      </c>
       <c r="G87">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="19" t="s">
-        <v>108</v>
-      </c>
+      <c r="A88" s="19"/>
       <c r="B88" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D88" s="18">
         <v>1</v>
       </c>
       <c r="E88" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G88">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="19" t="s">
-        <v>109</v>
-      </c>
+      <c r="A89" s="19"/>
       <c r="B89" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D89" s="18">
         <v>1</v>
       </c>
-      <c r="E89" s="15">
-        <v>0.01</v>
-      </c>
+      <c r="E89" s="15"/>
       <c r="G89">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B90" s="19" t="s">
         <v>94</v>
@@ -2839,14 +2866,16 @@
         <v>1</v>
       </c>
       <c r="E90" s="15">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="19"/>
+      <c r="A91" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="B91" s="19" t="s">
         <v>94</v>
       </c>
@@ -2857,11 +2886,16 @@
         <v>1</v>
       </c>
       <c r="E91" s="15">
-        <v>1</v>
+        <v>0.01</v>
+      </c>
+      <c r="G91">
+        <v>75</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="19"/>
+      <c r="A92" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="B92" s="19" t="s">
         <v>94</v>
       </c>
@@ -2871,111 +2905,108 @@
       <c r="D92" s="18">
         <v>1</v>
       </c>
-      <c r="E92" s="15"/>
+      <c r="E92" s="15">
+        <v>0.67</v>
+      </c>
       <c r="G92">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="19" t="s">
-        <v>59</v>
-      </c>
+      <c r="A93" s="19"/>
       <c r="B93" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D93" s="18">
-        <v>2</v>
-      </c>
-      <c r="E93" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="G93">
-        <v>78</v>
+        <v>1</v>
+      </c>
+      <c r="E93" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="19" t="s">
-        <v>60</v>
-      </c>
+      <c r="A94" s="19"/>
       <c r="B94" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D94" s="18">
-        <v>2</v>
-      </c>
-      <c r="E94" s="15">
-        <v>365</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E94" s="15"/>
       <c r="G94">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="19" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="B95" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D95" s="18">
         <v>2</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="G95">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B96" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D96" s="18">
         <v>2</v>
       </c>
       <c r="E96" s="15">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G96">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="19"/>
+      <c r="A97" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="B97" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D97" s="18">
         <v>2</v>
       </c>
-      <c r="E97" s="15">
-        <v>0.2</v>
+      <c r="E97" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="G97">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="19"/>
+      <c r="A98" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="B98" s="19" t="s">
         <v>94</v>
       </c>
@@ -2986,10 +3017,10 @@
         <v>2</v>
       </c>
       <c r="E98" s="15">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G98">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3004,10 +3035,10 @@
         <v>2</v>
       </c>
       <c r="E99" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G99">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3022,52 +3053,51 @@
         <v>2</v>
       </c>
       <c r="E100" s="15">
-        <v>1.69</v>
+        <v>0.5</v>
       </c>
       <c r="G100">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="A101" s="19"/>
       <c r="B101" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D101" s="18">
         <v>2</v>
       </c>
       <c r="E101" s="15">
-        <v>0</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G101">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="19" t="s">
-        <v>109</v>
-      </c>
+      <c r="A102" s="19"/>
       <c r="B102" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D102" s="18">
         <v>2</v>
       </c>
       <c r="E102" s="15">
-        <v>0</v>
+        <v>1.69</v>
+      </c>
+      <c r="G102">
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="19" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="B103" s="19" t="s">
         <v>94</v>
@@ -3079,11 +3109,16 @@
         <v>2</v>
       </c>
       <c r="E103" s="15">
-        <v>0.02</v>
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>86</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="19"/>
+      <c r="A104" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="B104" s="19" t="s">
         <v>94</v>
       </c>
@@ -3094,11 +3129,13 @@
         <v>2</v>
       </c>
       <c r="E104" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="19"/>
+      <c r="A105" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="B105" s="19" t="s">
         <v>94</v>
       </c>
@@ -3109,20 +3146,38 @@
         <v>2</v>
       </c>
       <c r="E105" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="19"/>
+      <c r="B106" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C106" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D106" s="18">
+        <v>2</v>
+      </c>
+      <c r="E106" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="20"/>
-      <c r="B106" s="20"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="22"/>
-    </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="20"/>
-      <c r="B107" s="20"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="22"/>
+      <c r="A107" s="19"/>
+      <c r="B107" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C107" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D107" s="18">
+        <v>2</v>
+      </c>
+      <c r="E107" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="20"/>
@@ -3774,11 +3829,13 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="20"/>
+      <c r="B216" s="20"/>
       <c r="C216" s="21"/>
       <c r="D216" s="22"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="20"/>
+      <c r="B217" s="20"/>
       <c r="C217" s="21"/>
       <c r="D217" s="22"/>
     </row>
@@ -3822,17 +3879,27 @@
       <c r="C225" s="21"/>
       <c r="D225" s="22"/>
     </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="20"/>
+      <c r="C226" s="21"/>
+      <c r="D226" s="22"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="20"/>
+      <c r="C227" s="21"/>
+      <c r="D227" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A37:A39"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="13">
@@ -3845,21 +3912,21 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{FCAB33B4-E22D-416A-9EE8-1B6629F4B7A9}">
       <formula1>"angiosperm, gymnosperm"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E78" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E80" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E27 E79 E74 E76:E77" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28 E81 E76 E78:E79" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E16" xr:uid="{89511D6B-7806-4594-AA02-B0D66F3A6A50}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E17" xr:uid="{89511D6B-7806-4594-AA02-B0D66F3A6A50}">
       <formula1>1</formula1>
       <formula2>366</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{5620C1FF-B28B-4556-ADEF-5FA98FE67CB9}">
       <formula1>"C3, C4, CAM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E18" xr:uid="{D43B937F-2CE8-47D9-A978-7D336015DF11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E19" xr:uid="{D43B937F-2CE8-47D9-A978-7D336015DF11}">
       <formula1>"Annual, Herbaceous perennial, Woody perennial"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{6E5E4A37-6A5B-480B-8E8F-63973FC4A36F}">
@@ -3874,7 +3941,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{793E17DF-C558-4DAF-B608-9E20297CD619}">
       <formula1>"annual, perennial evergreen, perennial deciduous"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E82 E95" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84 E97" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3885,10 +3952,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
-  <dimension ref="A1:N225"/>
+  <dimension ref="A1:N227"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B56" sqref="A56:XFD59"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4127,92 +4194,89 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>78</v>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="18"/>
+      <c r="C14" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="11"/>
       <c r="E14" s="15">
-        <v>180</v>
-      </c>
-      <c r="G14">
-        <v>50</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>137</v>
+        <v>78</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="15">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>23</v>
+        <v>180</v>
+      </c>
+      <c r="G15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>137</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="15">
+      <c r="D17" s="11"/>
+      <c r="E17" s="15">
         <v>273</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="8"/>
-      <c r="G17">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="8"/>
+      <c r="G18">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+    <row r="19" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" s="15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G18">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
       <c r="B19" s="9" t="s">
         <v>87</v>
       </c>
@@ -4220,13 +4284,13 @@
         <v>65</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E19" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G19">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -4238,13 +4302,13 @@
         <v>65</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E20" s="15">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G20">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -4256,37 +4320,37 @@
         <v>65</v>
       </c>
       <c r="D21" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="G21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
+      <c r="B22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E22" s="15">
         <v>0.01</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="15">
-        <v>1.444</v>
-      </c>
-      <c r="G22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
       <c r="B23" s="9" t="s">
         <v>87</v>
       </c>
@@ -4294,13 +4358,13 @@
         <v>27</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E23" s="15">
-        <v>1.5129999999999999</v>
+        <v>1.444</v>
       </c>
       <c r="G23">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -4312,13 +4376,13 @@
         <v>27</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E24" s="15">
-        <v>1.4630000000000001</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="G24">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4330,108 +4394,104 @@
         <v>27</v>
       </c>
       <c r="D25" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="15">
+        <v>1.4630000000000001</v>
+      </c>
+      <c r="G25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E26" s="15">
         <v>1.4139999999999999</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="10" t="s">
+      <c r="B27" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="15">
-        <v>0.48</v>
-      </c>
-      <c r="G26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="15">
-        <v>100</v>
-      </c>
-      <c r="F27" t="s">
-        <v>64</v>
+        <v>0.48</v>
       </c>
       <c r="G27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="15">
+        <v>100</v>
+      </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="15">
         <v>0.05</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:8" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:8" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30">
-        <v>27</v>
-      </c>
-      <c r="H30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
       <c r="B31" s="9" t="s">
         <v>87</v>
       </c>
@@ -4439,12 +4499,17 @@
         <v>95</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E31" s="15"/>
-      <c r="F31" s="31"/>
+      <c r="F31" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="G31">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="H31" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -4456,12 +4521,12 @@
         <v>95</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="31"/>
       <c r="G32">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -4470,15 +4535,15 @@
         <v>87</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="31"/>
       <c r="G33">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -4490,12 +4555,12 @@
         <v>96</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="31"/>
       <c r="G34">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -4507,36 +4572,35 @@
         <v>96</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35" s="15"/>
       <c r="F35" s="31"/>
       <c r="G35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="30"/>
+      <c r="B36" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="31"/>
+      <c r="G36">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="G36">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
       <c r="B37" s="9" t="s">
         <v>87</v>
       </c>
@@ -4544,14 +4608,13 @@
         <v>41</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" s="27">
-        <f>E38/0.27*0.2</f>
-        <v>2.2222222222222223E-2</v>
+        <v>98</v>
+      </c>
+      <c r="E37" s="15">
+        <v>0.01</v>
       </c>
       <c r="G37">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -4563,13 +4626,14 @@
         <v>41</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E38" s="15">
-        <v>0.03</v>
+        <v>99</v>
+      </c>
+      <c r="E38" s="27">
+        <f>E39/0.27*0.2</f>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="G38">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -4581,37 +4645,37 @@
         <v>41</v>
       </c>
       <c r="D39" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="G39">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="28"/>
+      <c r="B40" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E40" s="15">
         <v>0</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="15">
-        <v>4.3</v>
-      </c>
-      <c r="G40">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
       <c r="B41" s="9" t="s">
         <v>87</v>
       </c>
@@ -4619,29 +4683,13 @@
         <v>75</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E41" s="15">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="G41">
-        <v>39</v>
-      </c>
-      <c r="J41">
-        <f>E41+E42</f>
-        <v>9.6</v>
-      </c>
-      <c r="K41">
-        <f>LOG10(J41/1000)</f>
-        <v>-2.0177287669604316</v>
-      </c>
-      <c r="M41">
-        <f>E63/E64</f>
-        <v>2.5</v>
-      </c>
-      <c r="N41">
-        <f>LOG10(M41)</f>
-        <v>0.3979400086720376</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -4653,29 +4701,29 @@
         <v>75</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E42" s="15">
-        <v>5.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G42">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J42">
-        <f>(E37+E38)/E67*E63</f>
-        <v>0.52222222222222237</v>
+        <f>E42+E43</f>
+        <v>9.6</v>
       </c>
       <c r="K42">
         <f>LOG10(J42/1000)</f>
-        <v>-3.2821446515036072</v>
+        <v>-2.0177287669604316</v>
       </c>
       <c r="M42">
-        <f>E63/E68</f>
-        <v>138.2930051648863</v>
+        <f>E64/E65</f>
+        <v>2.5</v>
       </c>
       <c r="N42">
         <f>LOG10(M42)</f>
-        <v>2.1408002141287135</v>
+        <v>0.3979400086720376</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -4687,35 +4735,53 @@
         <v>75</v>
       </c>
       <c r="D43" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="G43">
+        <v>40</v>
+      </c>
+      <c r="J43">
+        <f>(E38+E39)/E68*E64</f>
+        <v>0.52222222222222237</v>
+      </c>
+      <c r="K43">
+        <f>LOG10(J43/1000)</f>
+        <v>-3.2821446515036072</v>
+      </c>
+      <c r="M43">
+        <f>E64/E69</f>
+        <v>138.2930051648863</v>
+      </c>
+      <c r="N43">
+        <f>LOG10(M43)</f>
+        <v>2.1408002141287135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="28"/>
+      <c r="B44" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E44" s="15">
         <v>4</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="16" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
       <c r="B45" s="9" t="s">
         <v>87</v>
       </c>
@@ -4723,7 +4789,7 @@
         <v>147</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E45" s="15"/>
       <c r="F45" s="16" t="s">
@@ -4739,7 +4805,7 @@
         <v>147</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="16" t="s">
@@ -4755,7 +4821,7 @@
         <v>147</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="16" t="s">
@@ -4763,17 +4829,15 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
-        <v>151</v>
-      </c>
+      <c r="A48" s="28"/>
       <c r="B48" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E48" s="15"/>
       <c r="F48" s="16" t="s">
@@ -4781,7 +4845,9 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+      <c r="A49" s="28" t="s">
+        <v>151</v>
+      </c>
       <c r="B49" s="9" t="s">
         <v>87</v>
       </c>
@@ -4789,7 +4855,7 @@
         <v>145</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E49" s="15"/>
       <c r="F49" s="16" t="s">
@@ -4805,7 +4871,7 @@
         <v>145</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E50" s="15"/>
       <c r="F50" s="16" t="s">
@@ -4821,7 +4887,7 @@
         <v>145</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="16" t="s">
@@ -4829,17 +4895,15 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
-        <v>152</v>
-      </c>
+      <c r="A52" s="28"/>
       <c r="B52" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E52" s="15"/>
       <c r="F52" s="16" t="s">
@@ -4847,7 +4911,9 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
+      <c r="A53" s="28" t="s">
+        <v>152</v>
+      </c>
       <c r="B53" s="9" t="s">
         <v>87</v>
       </c>
@@ -4855,7 +4921,7 @@
         <v>148</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E53" s="15"/>
       <c r="F53" s="16" t="s">
@@ -4871,7 +4937,7 @@
         <v>148</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E54" s="15"/>
       <c r="F54" s="16" t="s">
@@ -4887,7 +4953,7 @@
         <v>148</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="16" t="s">
@@ -4895,17 +4961,15 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
-        <v>153</v>
-      </c>
+      <c r="A56" s="28"/>
       <c r="B56" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="16" t="s">
@@ -4913,7 +4977,9 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
+      <c r="A57" s="28" t="s">
+        <v>153</v>
+      </c>
       <c r="B57" s="9" t="s">
         <v>87</v>
       </c>
@@ -4921,7 +4987,7 @@
         <v>154</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E57" s="15"/>
       <c r="F57" s="16" t="s">
@@ -4937,7 +5003,7 @@
         <v>154</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E58" s="15"/>
       <c r="F58" s="16" t="s">
@@ -4953,463 +5019,458 @@
         <v>154</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E59" s="15"/>
       <c r="F59" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="28"/>
+      <c r="B60" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E60" s="15"/>
+      <c r="F60" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="8"/>
-      <c r="J60">
-        <f>PI()/4*E64^2*E63</f>
+      <c r="B61" s="5"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="8"/>
+      <c r="J61">
+        <f>PI()/4*E65^2*E64</f>
         <v>5.3014376029327764E-2</v>
       </c>
-      <c r="K60">
-        <f>J41/1000/J60</f>
+      <c r="K61">
+        <f>J42/1000/J61</f>
         <v>0.18108295747344533</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+    <row r="62" spans="1:11" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
         <v>43</v>
-      </c>
-      <c r="B61" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="15">
-        <v>18</v>
-      </c>
-      <c r="I61">
-        <f>E63/E68</f>
-        <v>138.2930051648863</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="B62" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D62" s="18"/>
       <c r="E62" s="15">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="I62">
-        <f>E63/E64</f>
-        <v>2.5</v>
+        <f>E64/E69</f>
+        <v>138.2930051648863</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B63" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="D63" s="18"/>
       <c r="E63" s="15">
-        <v>0.75</v>
+        <v>10</v>
+      </c>
+      <c r="I63">
+        <f>E64/E65</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B64" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="D64" s="18"/>
       <c r="E64" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="G64">
-        <v>48</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B65" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="15">
-        <v>0.33</v>
+        <v>0.3</v>
+      </c>
+      <c r="G65">
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B66" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D66" s="18"/>
       <c r="E66" s="15">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B67" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D67" s="18"/>
       <c r="E67" s="15">
-        <f>E63/10</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="K67" t="e">
-        <f>(K60-K61)/K61</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M67" t="e">
-        <f>(M61-M60)/M61</f>
-        <v>#DIV/0!</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C68" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" s="18"/>
+      <c r="E68" s="15">
+        <f>E64/10</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K68" t="e">
+        <f>(K61-K62)/K62</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M68" t="e">
+        <f>(M62-M61)/M62</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="D68" s="18"/>
-      <c r="E68" s="27">
+      <c r="D69" s="18"/>
+      <c r="E69" s="27">
         <f>SQRT(0.231/100/100*4/PI())</f>
         <v>5.423267786434878E-3</v>
       </c>
-      <c r="G68">
+      <c r="G69">
         <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B69" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="D69" s="18"/>
-      <c r="E69" s="15">
-        <v>0.02</v>
-      </c>
-      <c r="G69">
-        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D70" s="18"/>
       <c r="E70" s="15">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G70">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B71" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="18"/>
+      <c r="E71" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G71">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A72" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="15">
+        <v>7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="D71" s="19"/>
-      <c r="E71" s="15">
+      <c r="D73" s="19"/>
+      <c r="E73" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" t="s">
         <v>122</v>
       </c>
-      <c r="G71">
+      <c r="G73">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="5" t="s">
+    <row r="74" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="8"/>
-      <c r="G72">
+      <c r="B74" s="5"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="8"/>
+      <c r="G74">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+    <row r="75" spans="1:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="B73" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D73" s="18"/>
-      <c r="E73" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="G73">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B74" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G74">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
-        <v>121</v>
       </c>
       <c r="B75" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="D75" s="18"/>
       <c r="E75" s="15">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
       <c r="G75">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" s="18"/>
+      <c r="E76" s="15">
+        <v>0.5</v>
       </c>
       <c r="G76">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="G77">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G78">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B79" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D79" s="18"/>
+      <c r="E79" s="15">
         <v>0.01</v>
       </c>
-      <c r="G77">
+      <c r="G79">
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
+    <row r="80" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="B80" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="C80" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D78" s="18"/>
-      <c r="E78" s="15">
+      <c r="D80" s="18"/>
+      <c r="E80" s="15">
         <v>365</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F80" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="5" t="s">
+    <row r="81" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="8"/>
-      <c r="G79">
+      <c r="B81" s="5"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="8"/>
+      <c r="G81">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
+    <row r="82" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C80" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D80" s="18">
-        <v>1</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G80">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D81" s="18">
-        <v>1</v>
-      </c>
-      <c r="E81" s="15">
-        <v>207</v>
-      </c>
-      <c r="G81">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
-        <v>102</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D82" s="18">
         <v>1</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="G82">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D83" s="18">
         <v>1</v>
       </c>
       <c r="E83" s="15">
-        <v>30</v>
+        <v>207</v>
       </c>
       <c r="G83">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="19"/>
+      <c r="A84" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="B84" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D84" s="18">
         <v>1</v>
       </c>
-      <c r="E84" s="15">
-        <v>40</v>
+      <c r="E84" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="G84">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="19"/>
+      <c r="A85" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="B85" s="19" t="s">
         <v>94</v>
       </c>
@@ -5420,10 +5481,10 @@
         <v>1</v>
       </c>
       <c r="E85" s="15">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G85">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -5438,10 +5499,10 @@
         <v>1</v>
       </c>
       <c r="E86" s="15">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="G86">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -5455,29 +5516,29 @@
       <c r="D87" s="18">
         <v>1</v>
       </c>
-      <c r="E87" s="15"/>
+      <c r="E87" s="15">
+        <v>50</v>
+      </c>
       <c r="G87">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="19" t="s">
-        <v>58</v>
-      </c>
+      <c r="A88" s="19"/>
       <c r="B88" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D88" s="18">
         <v>1</v>
       </c>
       <c r="E88" s="15">
-        <v>0.01</v>
+        <v>55</v>
       </c>
       <c r="G88">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -5486,20 +5547,20 @@
         <v>94</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D89" s="18">
         <v>1</v>
       </c>
-      <c r="E89" s="15">
-        <v>0.25</v>
-      </c>
+      <c r="E89" s="15"/>
       <c r="G89">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="19"/>
+      <c r="A90" s="19" t="s">
+        <v>58</v>
+      </c>
       <c r="B90" s="19" t="s">
         <v>94</v>
       </c>
@@ -5510,10 +5571,10 @@
         <v>1</v>
       </c>
       <c r="E90" s="15">
-        <v>0.67</v>
+        <v>0.01</v>
       </c>
       <c r="G90">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -5528,10 +5589,10 @@
         <v>1</v>
       </c>
       <c r="E91" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="F91" t="s">
-        <v>107</v>
+        <v>0.25</v>
+      </c>
+      <c r="G91">
+        <v>75</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -5545,111 +5606,111 @@
       <c r="D92" s="18">
         <v>1</v>
       </c>
-      <c r="E92" s="15"/>
+      <c r="E92" s="15">
+        <v>0.67</v>
+      </c>
       <c r="G92">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="19" t="s">
-        <v>59</v>
-      </c>
+      <c r="A93" s="19"/>
       <c r="B93" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D93" s="18">
-        <v>2</v>
-      </c>
-      <c r="E93" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="G93">
-        <v>78</v>
+        <v>1</v>
+      </c>
+      <c r="E93" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F93" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="19" t="s">
-        <v>60</v>
-      </c>
+      <c r="A94" s="19"/>
       <c r="B94" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D94" s="18">
-        <v>2</v>
-      </c>
-      <c r="E94" s="15">
-        <v>365</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E94" s="15"/>
       <c r="G94">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="19" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="B95" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D95" s="18">
         <v>2</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="G95">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B96" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D96" s="18">
         <v>2</v>
       </c>
       <c r="E96" s="15">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G96">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="19"/>
+      <c r="A97" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="B97" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D97" s="18">
         <v>2</v>
       </c>
-      <c r="E97" s="15">
-        <v>0.5</v>
+      <c r="E97" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="G97">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="19"/>
+      <c r="A98" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="B98" s="19" t="s">
         <v>94</v>
       </c>
@@ -5660,10 +5721,10 @@
         <v>2</v>
       </c>
       <c r="E98" s="15">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G98">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -5678,10 +5739,10 @@
         <v>2</v>
       </c>
       <c r="E99" s="15">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="G99">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -5696,30 +5757,28 @@
         <v>2</v>
       </c>
       <c r="E100" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="G100">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="A101" s="19"/>
       <c r="B101" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D101" s="18">
         <v>2</v>
       </c>
       <c r="E101" s="15">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="G101">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -5728,17 +5787,22 @@
         <v>94</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D102" s="18">
         <v>2</v>
       </c>
       <c r="E102" s="15">
-        <v>0</v>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G102">
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="19"/>
+      <c r="A103" s="19" t="s">
+        <v>62</v>
+      </c>
       <c r="B103" s="19" t="s">
         <v>94</v>
       </c>
@@ -5749,7 +5813,10 @@
         <v>2</v>
       </c>
       <c r="E103" s="15">
-        <v>0.3</v>
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>86</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -5764,7 +5831,7 @@
         <v>2</v>
       </c>
       <c r="E104" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -5779,20 +5846,38 @@
         <v>2</v>
       </c>
       <c r="E105" s="15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="19"/>
+      <c r="B106" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C106" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D106" s="18">
+        <v>2</v>
+      </c>
+      <c r="E106" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="20"/>
-      <c r="B106" s="20"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="22"/>
-    </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="20"/>
-      <c r="B107" s="20"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="22"/>
+      <c r="A107" s="19"/>
+      <c r="B107" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C107" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D107" s="18">
+        <v>2</v>
+      </c>
+      <c r="E107" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="20"/>
@@ -6502,35 +6587,47 @@
       <c r="C225" s="21"/>
       <c r="D225" s="22"/>
     </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="20"/>
+      <c r="B226" s="20"/>
+      <c r="C226" s="21"/>
+      <c r="D226" s="22"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="20"/>
+      <c r="B227" s="20"/>
+      <c r="C227" s="21"/>
+      <c r="D227" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="F30:F35"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="F31:F36"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A53:A56"/>
   </mergeCells>
   <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E17 E29" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E18 E30" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
       <formula1>"Annual, Herbaceous perennial, Woody perennial"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{BF09F0A8-DEDC-4564-B7AE-B6347D314DF5}">
       <formula1>"C3, C4, CAM"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E16" xr:uid="{2135F1C0-D38D-4F5D-8EF7-81232862BF29}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E17" xr:uid="{2135F1C0-D38D-4F5D-8EF7-81232862BF29}">
       <formula1>1</formula1>
       <formula2>366</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26 E79 E74 E76:E77" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E27 E81 E76 E78:E79" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E78" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E80" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{9966BE53-3AF7-47D9-9DC3-79C6924CF42E}">
@@ -6554,7 +6651,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9" xr:uid="{82D88EBD-3D9A-4158-A9B3-F883994282C6}">
       <formula1>"climbing,columnar,conical,decumbent,erect,irregular,oval,prostrate,rounded,semi_erect,vase"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E82 E95" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84 E97" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Edited photosynthesis to calc gphot from leaf area
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF666285-C08E-47E4-AF22-5BF476D6D893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8152E0-9D4C-4EC1-A870-272316836A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-16190" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="-19200" yWindow="-16190" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
     <sheet name="BTS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1226,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
   <dimension ref="A1:M227"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:XFD72"/>
+    <sheetView topLeftCell="A22" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,15 +2127,15 @@
       </c>
       <c r="I49">
         <f>E64/E65</f>
-        <v>4.6550000000000002</v>
+        <v>3.0032258064516131</v>
       </c>
       <c r="J49">
         <f>E64/E65</f>
-        <v>4.6550000000000002</v>
+        <v>3.0032258064516131</v>
       </c>
       <c r="K49">
         <f>LOG10(J49)</f>
-        <v>0.66791968531736146</v>
+        <v>0.47758798714706996</v>
       </c>
       <c r="M49">
         <f>LOG10((E42+E43)/1000)</f>
@@ -2158,11 +2159,11 @@
       </c>
       <c r="J50">
         <f>E69/E68</f>
-        <v>0.375</v>
+        <v>0.5625</v>
       </c>
       <c r="K50">
         <f>LOG10(J50)</f>
-        <v>-0.42596873227228116</v>
+        <v>-0.24987747321659989</v>
       </c>
       <c r="M50">
         <f>LOG10((E38+E39)/1000)</f>
@@ -2202,7 +2203,7 @@
       </c>
       <c r="J52">
         <f>(E42+E43)/1000/(E64*PI()/4*E65^2)</f>
-        <v>0.57097476898703581</v>
+        <v>0.23765859271052481</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -2224,11 +2225,11 @@
       </c>
       <c r="I53">
         <f>E64/E69</f>
-        <v>15.516666666666667</v>
+        <v>10.344444444444445</v>
       </c>
       <c r="J53">
         <f>(E38+E39)/1000/(E68*PI()/4*E69^2)</f>
-        <v>1.5473397245045379</v>
+        <v>0.68770654422423905</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -2280,7 +2281,7 @@
       </c>
       <c r="K56">
         <f>(K49-K50)/K50</f>
-        <v>-2.5680016741003988</v>
+        <v>-2.9112886848070736</v>
       </c>
       <c r="M56">
         <f>(M50-M49)/M50</f>
@@ -2424,7 +2425,8 @@
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="15">
-        <v>0.2</v>
+        <f>0.31</f>
+        <v>0.31</v>
       </c>
       <c r="G65">
         <v>48</v>
@@ -2487,7 +2489,8 @@
       </c>
       <c r="D69" s="18"/>
       <c r="E69" s="15">
-        <v>0.06</v>
+        <f>0.09</f>
+        <v>0.09</v>
       </c>
       <c r="G69">
         <v>49</v>
@@ -3954,8 +3957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
   <dimension ref="A1:N227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4745,11 +4748,11 @@
       </c>
       <c r="J43">
         <f>(E38+E39)/E68*E64</f>
-        <v>0.52222222222222237</v>
+        <v>5.2222222222222225E-2</v>
       </c>
       <c r="K43">
         <f>LOG10(J43/1000)</f>
-        <v>-3.2821446515036072</v>
+        <v>-4.2821446515036072</v>
       </c>
       <c r="M43">
         <f>E64/E69</f>
@@ -5125,6 +5128,7 @@
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="15">
+        <f>0.3</f>
         <v>0.3</v>
       </c>
       <c r="G65">
@@ -5173,8 +5177,8 @@
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="15">
-        <f>E64/10</f>
-        <v>7.4999999999999997E-2</v>
+        <f>E64</f>
+        <v>0.75</v>
       </c>
       <c r="K68" t="e">
         <f>(K61-K62)/K62</f>
@@ -6601,16 +6605,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A53:A56"/>
     <mergeCell ref="F31:F36"/>
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A53:A56"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E18 E30" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">

</xml_diff>

<commit_message>
summed dead leaf biomass and removed from leaf, added lai crit to inputs
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8152E0-9D4C-4EC1-A870-272316836A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC7484C-0585-4700-8A20-64B9BDFD67DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="-16190" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
     <sheet name="BTS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="162">
   <si>
     <t>Parameter</t>
   </si>
@@ -674,6 +673,15 @@
   </si>
   <si>
     <t>sp_leaf_area</t>
+  </si>
+  <si>
+    <t>Critical LAI for self-pruning</t>
+  </si>
+  <si>
+    <t>lai_cr</t>
+  </si>
+  <si>
+    <t>This is the critical LAI above which leaf death starts to occur</t>
   </si>
 </sst>
 </file>
@@ -1225,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
-  <dimension ref="A1:M227"/>
+  <dimension ref="A1:M228"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,225 +2576,225 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D74" s="19"/>
+      <c r="E74" s="15">
+        <v>4</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="8"/>
-      <c r="G74">
+      <c r="B75" s="5"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="8"/>
+      <c r="G75">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
+    <row r="76" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="B75" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="15">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="G75">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="15">
-        <v>0.5</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="G76">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G77">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" s="18"/>
+      <c r="E78" s="15">
         <f>20*0.2*0.69</f>
         <v>2.76</v>
       </c>
-      <c r="F77" s="8" t="s">
+      <c r="F78" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G77">
+      <c r="G78">
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="5" t="s">
+    <row r="79" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="6"/>
-      <c r="F78" t="s">
+      <c r="B79" s="5"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="6"/>
+      <c r="F79" t="s">
         <v>101</v>
       </c>
-      <c r="G78">
+      <c r="G79">
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+    <row r="80" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="B79" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="18"/>
-      <c r="E79" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="F79" t="s">
-        <v>106</v>
-      </c>
-      <c r="G79">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
-        <v>50</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>89</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D80" s="18"/>
       <c r="E80" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F80" t="s">
+        <v>106</v>
+      </c>
+      <c r="G80">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" s="18"/>
+      <c r="E81" s="15">
         <v>365</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F81" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+    <row r="82" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="6"/>
-      <c r="G81">
+      <c r="B82" s="5"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="6"/>
+      <c r="G82">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+    <row r="83" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D82" s="18">
-        <v>1</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G82">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
-        <v>56</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D83" s="18">
         <v>1</v>
       </c>
-      <c r="E83" s="15">
-        <v>207</v>
+      <c r="E83" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="G83">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="D84" s="18">
         <v>1</v>
       </c>
-      <c r="E84" s="12" t="s">
-        <v>104</v>
+      <c r="E84" s="15">
+        <v>207</v>
       </c>
       <c r="G84">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B85" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D85" s="18">
         <v>1</v>
       </c>
-      <c r="E85">
-        <v>20</v>
+      <c r="E85" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="G85">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="19"/>
+      <c r="A86" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="B86" s="19" t="s">
         <v>94</v>
       </c>
@@ -2796,11 +2804,11 @@
       <c r="D86" s="18">
         <v>1</v>
       </c>
-      <c r="E86" s="15">
-        <v>30</v>
+      <c r="E86">
+        <v>20</v>
       </c>
       <c r="G86">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2815,10 +2823,10 @@
         <v>1</v>
       </c>
       <c r="E87" s="15">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="G87">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2833,10 +2841,10 @@
         <v>1</v>
       </c>
       <c r="E88" s="15">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G88">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2850,34 +2858,32 @@
       <c r="D89" s="18">
         <v>1</v>
       </c>
-      <c r="E89" s="15"/>
+      <c r="E89" s="15">
+        <v>100</v>
+      </c>
       <c r="G89">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="19" t="s">
-        <v>108</v>
-      </c>
+      <c r="A90" s="19"/>
       <c r="B90" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D90" s="18">
         <v>1</v>
       </c>
-      <c r="E90" s="15">
-        <v>0</v>
-      </c>
+      <c r="E90" s="15"/>
       <c r="G90">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>94</v>
@@ -2889,15 +2895,15 @@
         <v>1</v>
       </c>
       <c r="E91" s="15">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G91">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B92" s="19" t="s">
         <v>94</v>
@@ -2909,14 +2915,16 @@
         <v>1</v>
       </c>
       <c r="E92" s="15">
-        <v>0.67</v>
+        <v>0.01</v>
       </c>
       <c r="G92">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="19"/>
+      <c r="A93" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="B93" s="19" t="s">
         <v>94</v>
       </c>
@@ -2927,7 +2935,10 @@
         <v>1</v>
       </c>
       <c r="E93" s="15">
-        <v>1</v>
+        <v>0.67</v>
+      </c>
+      <c r="G93">
+        <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -2941,93 +2952,90 @@
       <c r="D94" s="18">
         <v>1</v>
       </c>
-      <c r="E94" s="15"/>
-      <c r="G94">
-        <v>77</v>
+      <c r="E94" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="19" t="s">
-        <v>59</v>
-      </c>
+      <c r="A95" s="19"/>
       <c r="B95" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D95" s="18">
-        <v>2</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>141</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E95" s="15"/>
       <c r="G95">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B96" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D96" s="18">
         <v>2</v>
       </c>
-      <c r="E96" s="15">
-        <v>365</v>
+      <c r="E96" s="12" t="s">
+        <v>141</v>
       </c>
       <c r="G96">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="19" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="B97" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="D97" s="18">
         <v>2</v>
       </c>
-      <c r="E97" s="12" t="s">
-        <v>104</v>
+      <c r="E97" s="15">
+        <v>365</v>
       </c>
       <c r="G97">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="19" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="B98" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D98" s="18">
         <v>2</v>
       </c>
-      <c r="E98" s="15">
-        <v>0</v>
+      <c r="E98" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="G98">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="19"/>
+      <c r="A99" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="B99" s="19" t="s">
         <v>94</v>
       </c>
@@ -3038,10 +3046,10 @@
         <v>2</v>
       </c>
       <c r="E99" s="15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G99">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3056,10 +3064,10 @@
         <v>2</v>
       </c>
       <c r="E100" s="15">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G100">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3074,10 +3082,10 @@
         <v>2</v>
       </c>
       <c r="E101" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="G101">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3092,35 +3100,33 @@
         <v>2</v>
       </c>
       <c r="E102" s="15">
-        <v>1.69</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G102">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="A103" s="19"/>
       <c r="B103" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D103" s="18">
         <v>2</v>
       </c>
       <c r="E103" s="15">
-        <v>0</v>
+        <v>1.69</v>
       </c>
       <c r="G103">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="19" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="B104" s="19" t="s">
         <v>94</v>
@@ -3134,10 +3140,13 @@
       <c r="E104" s="15">
         <v>0</v>
       </c>
+      <c r="G104">
+        <v>86</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B105" s="19" t="s">
         <v>94</v>
@@ -3149,11 +3158,13 @@
         <v>2</v>
       </c>
       <c r="E105" s="15">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="19"/>
+      <c r="A106" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="B106" s="19" t="s">
         <v>94</v>
       </c>
@@ -3164,7 +3175,7 @@
         <v>2</v>
       </c>
       <c r="E106" s="15">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3183,10 +3194,19 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="20"/>
-      <c r="B108" s="20"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="22"/>
+      <c r="A108" s="19"/>
+      <c r="B108" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D108" s="18">
+        <v>2</v>
+      </c>
+      <c r="E108" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="20"/>
@@ -3844,6 +3864,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="20"/>
+      <c r="B218" s="20"/>
       <c r="C218" s="21"/>
       <c r="D218" s="22"/>
     </row>
@@ -3891,6 +3912,11 @@
       <c r="A227" s="20"/>
       <c r="C227" s="21"/>
       <c r="D227" s="22"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="20"/>
+      <c r="C228" s="21"/>
+      <c r="D228" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3915,10 +3941,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{FCAB33B4-E22D-416A-9EE8-1B6629F4B7A9}">
       <formula1>"angiosperm, gymnosperm"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E80" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E81" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28 E81 E76 E78:E79" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28 E82 E77 E79:E80" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -3944,7 +3970,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{793E17DF-C558-4DAF-B608-9E20297CD619}">
       <formula1>"annual, perennial evergreen, perennial deciduous"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84 E97" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E85 E98" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3955,10 +3981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
-  <dimension ref="A1:N227"/>
+  <dimension ref="A1:N228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5280,219 +5306,219 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D74" s="19"/>
+      <c r="E74" s="15">
+        <v>4</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="8"/>
-      <c r="G74">
+      <c r="B75" s="5"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="8"/>
+      <c r="G75">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
+    <row r="76" spans="1:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="B75" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="G75">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G76">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G77">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" s="18"/>
+      <c r="E78" s="15">
         <v>1.2</v>
       </c>
-      <c r="G77">
+      <c r="G78">
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="5" t="s">
+    <row r="79" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="8" t="s">
+      <c r="B79" s="5"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G78">
+      <c r="G79">
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+    <row r="80" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="B79" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="18"/>
-      <c r="E79" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="G79">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
-        <v>50</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>89</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D80" s="18"/>
       <c r="E80" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G80">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" s="18"/>
+      <c r="E81" s="15">
         <v>365</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F81" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+    <row r="82" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="8"/>
-      <c r="G81">
+      <c r="B82" s="5"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="8"/>
+      <c r="G82">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+    <row r="83" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D82" s="18">
-        <v>1</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G82">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
-        <v>56</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D83" s="18">
         <v>1</v>
       </c>
-      <c r="E83" s="15">
-        <v>207</v>
+      <c r="E83" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="G83">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="D84" s="18">
         <v>1</v>
       </c>
-      <c r="E84" s="12" t="s">
-        <v>104</v>
+      <c r="E84" s="15">
+        <v>207</v>
       </c>
       <c r="G84">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B85" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D85" s="18">
         <v>1</v>
       </c>
-      <c r="E85" s="15">
-        <v>30</v>
+      <c r="E85" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="G85">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="19"/>
+      <c r="A86" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="B86" s="19" t="s">
         <v>94</v>
       </c>
@@ -5503,10 +5529,10 @@
         <v>1</v>
       </c>
       <c r="E86" s="15">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G86">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -5521,10 +5547,10 @@
         <v>1</v>
       </c>
       <c r="E87" s="15">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G87">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -5539,10 +5565,10 @@
         <v>1</v>
       </c>
       <c r="E88" s="15">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G88">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -5556,33 +5582,33 @@
       <c r="D89" s="18">
         <v>1</v>
       </c>
-      <c r="E89" s="15"/>
+      <c r="E89" s="15">
+        <v>55</v>
+      </c>
       <c r="G89">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="19" t="s">
-        <v>58</v>
-      </c>
+      <c r="A90" s="19"/>
       <c r="B90" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D90" s="18">
         <v>1</v>
       </c>
-      <c r="E90" s="15">
-        <v>0.01</v>
-      </c>
+      <c r="E90" s="15"/>
       <c r="G90">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="19"/>
+      <c r="A91" s="19" t="s">
+        <v>58</v>
+      </c>
       <c r="B91" s="19" t="s">
         <v>94</v>
       </c>
@@ -5593,10 +5619,10 @@
         <v>1</v>
       </c>
       <c r="E91" s="15">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="G91">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -5611,10 +5637,10 @@
         <v>1</v>
       </c>
       <c r="E92" s="15">
-        <v>0.67</v>
+        <v>0.25</v>
       </c>
       <c r="G92">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -5629,10 +5655,10 @@
         <v>1</v>
       </c>
       <c r="E93" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="F93" t="s">
-        <v>107</v>
+        <v>0.67</v>
+      </c>
+      <c r="G93">
+        <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -5646,93 +5672,93 @@
       <c r="D94" s="18">
         <v>1</v>
       </c>
-      <c r="E94" s="15"/>
-      <c r="G94">
-        <v>77</v>
+      <c r="E94" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F94" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="19" t="s">
-        <v>59</v>
-      </c>
+      <c r="A95" s="19"/>
       <c r="B95" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D95" s="18">
-        <v>2</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>141</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E95" s="15"/>
       <c r="G95">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B96" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D96" s="18">
         <v>2</v>
       </c>
-      <c r="E96" s="15">
-        <v>365</v>
+      <c r="E96" s="12" t="s">
+        <v>141</v>
       </c>
       <c r="G96">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="19" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="B97" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="D97" s="18">
         <v>2</v>
       </c>
-      <c r="E97" s="12" t="s">
-        <v>104</v>
+      <c r="E97" s="15">
+        <v>365</v>
       </c>
       <c r="G97">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="19" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="B98" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D98" s="18">
         <v>2</v>
       </c>
-      <c r="E98" s="15">
-        <v>0</v>
+      <c r="E98" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="G98">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="19"/>
+      <c r="A99" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="B99" s="19" t="s">
         <v>94</v>
       </c>
@@ -5743,10 +5769,10 @@
         <v>2</v>
       </c>
       <c r="E99" s="15">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G99">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -5761,10 +5787,10 @@
         <v>2</v>
       </c>
       <c r="E100" s="15">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G100">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -5779,10 +5805,10 @@
         <v>2</v>
       </c>
       <c r="E101" s="15">
-        <v>0.68</v>
+        <v>0.6</v>
       </c>
       <c r="G101">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -5797,34 +5823,34 @@
         <v>2</v>
       </c>
       <c r="E102" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="G102">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="A103" s="19"/>
       <c r="B103" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D103" s="18">
         <v>2</v>
       </c>
       <c r="E103" s="15">
-        <v>0</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G103">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="19"/>
+      <c r="A104" s="19" t="s">
+        <v>62</v>
+      </c>
       <c r="B104" s="19" t="s">
         <v>94</v>
       </c>
@@ -5836,6 +5862,9 @@
       </c>
       <c r="E104" s="15">
         <v>0</v>
+      </c>
+      <c r="G104">
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -5850,7 +5879,7 @@
         <v>2</v>
       </c>
       <c r="E105" s="15">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -5865,7 +5894,7 @@
         <v>2</v>
       </c>
       <c r="E106" s="15">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -5884,10 +5913,19 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="20"/>
-      <c r="B108" s="20"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="22"/>
+      <c r="A108" s="19"/>
+      <c r="B108" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D108" s="18">
+        <v>2</v>
+      </c>
+      <c r="E108" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="20"/>
@@ -6603,8 +6641,17 @@
       <c r="C227" s="21"/>
       <c r="D227" s="22"/>
     </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="20"/>
+      <c r="B228" s="20"/>
+      <c r="C228" s="21"/>
+      <c r="D228" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="A49:A52"/>
@@ -6612,9 +6659,6 @@
     <mergeCell ref="F31:F36"/>
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E18 E30" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
@@ -6627,11 +6671,11 @@
       <formula1>1</formula1>
       <formula2>366</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E27 E81 E76 E78:E79" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E27 E82 E77 E79:E80" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E80" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E81" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{9966BE53-3AF7-47D9-9DC3-79C6924CF42E}">
@@ -6655,7 +6699,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9" xr:uid="{82D88EBD-3D9A-4158-A9B3-F883994282C6}">
       <formula1>"climbing,columnar,conical,decumbent,erect,irregular,oval,prostrate,rounded,semi_erect,vase"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84 E97" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E85 E98" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added more checks for nans and infs throughout
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC7484C-0585-4700-8A20-64B9BDFD67DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29E1654-CDE2-4AA0-9E0A-C9E139BD06C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
@@ -675,13 +675,13 @@
     <t>sp_leaf_area</t>
   </si>
   <si>
-    <t>Critical LAI for self-pruning</t>
+    <t>Critical leaf area index</t>
   </si>
   <si>
     <t>lai_cr</t>
   </si>
   <si>
-    <t>This is the critical LAI above which leaf death starts to occur</t>
+    <t>Critical LAI before leaf death starts</t>
   </si>
 </sst>
 </file>
@@ -1235,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
   <dimension ref="A1:M228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,15 +2135,15 @@
       </c>
       <c r="I49">
         <f>E64/E65</f>
-        <v>3.0032258064516131</v>
+        <v>4.6550000000000002</v>
       </c>
       <c r="J49">
         <f>E64/E65</f>
-        <v>3.0032258064516131</v>
+        <v>4.6550000000000002</v>
       </c>
       <c r="K49">
         <f>LOG10(J49)</f>
-        <v>0.47758798714706996</v>
+        <v>0.66791968531736146</v>
       </c>
       <c r="M49">
         <f>LOG10((E42+E43)/1000)</f>
@@ -2167,11 +2167,11 @@
       </c>
       <c r="J50">
         <f>E69/E68</f>
-        <v>0.5625</v>
+        <v>0.375</v>
       </c>
       <c r="K50">
         <f>LOG10(J50)</f>
-        <v>-0.24987747321659989</v>
+        <v>-0.42596873227228116</v>
       </c>
       <c r="M50">
         <f>LOG10((E38+E39)/1000)</f>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="J52">
         <f>(E42+E43)/1000/(E64*PI()/4*E65^2)</f>
-        <v>0.23765859271052481</v>
+        <v>0.57097476898703581</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -2233,11 +2233,11 @@
       </c>
       <c r="I53">
         <f>E64/E69</f>
-        <v>10.344444444444445</v>
+        <v>15.516666666666667</v>
       </c>
       <c r="J53">
         <f>(E38+E39)/1000/(E68*PI()/4*E69^2)</f>
-        <v>0.68770654422423905</v>
+        <v>1.5473397245045379</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="K56">
         <f>(K49-K50)/K50</f>
-        <v>-2.9112886848070736</v>
+        <v>-2.5680016741003988</v>
       </c>
       <c r="M56">
         <f>(M50-M49)/M50</f>
@@ -2433,8 +2433,7 @@
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="15">
-        <f>0.31</f>
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="G65">
         <v>48</v>
@@ -2497,8 +2496,7 @@
       </c>
       <c r="D69" s="18"/>
       <c r="E69" s="15">
-        <f>0.09</f>
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="G69">
         <v>49</v>
@@ -3983,7 +3981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
   <dimension ref="A1:N228"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
+    <sheetView topLeftCell="A59" workbookViewId="0">
       <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
@@ -4774,11 +4772,11 @@
       </c>
       <c r="J43">
         <f>(E38+E39)/E68*E64</f>
-        <v>5.2222222222222225E-2</v>
+        <v>0.52222222222222237</v>
       </c>
       <c r="K43">
         <f>LOG10(J43/1000)</f>
-        <v>-4.2821446515036072</v>
+        <v>-3.2821446515036072</v>
       </c>
       <c r="M43">
         <f>E64/E69</f>
@@ -5154,7 +5152,6 @@
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="15">
-        <f>0.3</f>
         <v>0.3</v>
       </c>
       <c r="G65">
@@ -5203,8 +5200,8 @@
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="15">
-        <f>E64</f>
-        <v>0.75</v>
+        <f>E64/10</f>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="K68" t="e">
         <f>(K61-K62)/K62</f>
@@ -6649,9 +6646,6 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="A49:A52"/>
@@ -6659,6 +6653,9 @@
     <mergeCell ref="F31:F36"/>
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E18 E30" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">

</xml_diff>

<commit_message>
Updated photo testing and fixed nsc bug
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A816A29-6DA9-4EDD-8C40-06B8FBF8F07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92704FB-6B8B-4CFA-82DD-2A241E82FFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="177">
   <si>
     <t>Parameter</t>
   </si>
@@ -731,9 +731,6 @@
     </r>
   </si>
   <si>
-    <t>Teh uses 2600 which is &gt;&gt; tau reported in other pubs on rubisco limitation, 85 seems to be close to a reported value for several species</t>
-  </si>
-  <si>
     <t>ci</t>
   </si>
   <si>
@@ -741,6 +738,46 @@
   </si>
   <si>
     <t>spec_factor_25</t>
+  </si>
+  <si>
+    <t>stomatal_conductance</t>
+  </si>
+  <si>
+    <t>Stomatal conductance (mol/m2/s)</t>
+  </si>
+  <si>
+    <t>Maximum photosynthetic carboxylation rate (μmol/mol)</t>
+  </si>
+  <si>
+    <t>Typically reported in μmol/mol but can be reported in any consistent unuts</t>
+  </si>
+  <si>
+    <r>
+      <t>Base intercellular CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> concentration</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -902,7 +939,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -980,6 +1017,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1319,15 +1359,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
-  <dimension ref="A1:M233"/>
+  <dimension ref="A1:M234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A6" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41" style="23" customWidth="1"/>
+    <col min="1" max="1" width="54" style="23" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="23" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" style="15" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="24" customWidth="1"/>
@@ -1657,7 +1697,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>162</v>
@@ -1667,7 +1707,7 @@
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="15">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1684,6 +1724,9 @@
       <c r="E21" s="15">
         <v>11</v>
       </c>
+      <c r="F21" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
@@ -1699,23 +1742,26 @@
       <c r="E22" s="15">
         <v>300</v>
       </c>
+      <c r="F22" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>162</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="15">
         <v>300</v>
       </c>
       <c r="G23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1741,48 +1787,42 @@
         <v>162</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="15">
         <v>85</v>
       </c>
-      <c r="G25" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G27">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
       <c r="B28" s="9" t="s">
         <v>80</v>
       </c>
@@ -1790,17 +1830,17 @@
         <v>58</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E28" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G28">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="9" t="s">
         <v>80</v>
       </c>
@@ -1808,17 +1848,17 @@
         <v>58</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E29" s="15">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G29">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="9" t="s">
         <v>80</v>
       </c>
@@ -1826,37 +1866,37 @@
         <v>58</v>
       </c>
       <c r="D30" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="G30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E31" s="15">
         <v>0.01</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" s="15">
-        <v>1.444</v>
-      </c>
-      <c r="G31">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
       <c r="B32" s="9" t="s">
         <v>80</v>
       </c>
@@ -1864,17 +1904,17 @@
         <v>27</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E32" s="15">
-        <v>1.5129999999999999</v>
+        <v>1.444</v>
       </c>
       <c r="G32">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="A33" s="33"/>
       <c r="B33" s="9" t="s">
         <v>80</v>
       </c>
@@ -1882,17 +1922,17 @@
         <v>27</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E33" s="15">
-        <v>1.4630000000000001</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="G33">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="9" t="s">
         <v>80</v>
       </c>
@@ -1900,51 +1940,47 @@
         <v>27</v>
       </c>
       <c r="D34" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="15">
+        <v>1.4630000000000001</v>
+      </c>
+      <c r="G34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E35" s="15">
         <v>1.4139999999999999</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:13" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36">
-        <v>27</v>
-      </c>
-      <c r="H36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
       <c r="B37" s="9" t="s">
         <v>80</v>
       </c>
@@ -1952,15 +1988,21 @@
         <v>88</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E37" s="15"/>
+      <c r="F37" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="G37">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="H37" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="9" t="s">
         <v>80</v>
       </c>
@@ -1968,31 +2010,31 @@
         <v>88</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E38" s="15"/>
       <c r="G38">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E39" s="15"/>
       <c r="G39">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="9" t="s">
         <v>80</v>
       </c>
@@ -2000,15 +2042,15 @@
         <v>89</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E40" s="15"/>
       <c r="G40">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="9" t="s">
         <v>80</v>
       </c>
@@ -2016,51 +2058,33 @@
         <v>89</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E41" s="15"/>
       <c r="G41">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
+      <c r="B42" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="G42">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="G42">
-        <v>33</v>
-      </c>
-      <c r="J42">
-        <f>E44+E43</f>
-        <v>0.7</v>
-      </c>
-      <c r="K42">
-        <f>LOG10(J42/1000)</f>
-        <v>-3.1549019599857431</v>
-      </c>
-      <c r="L42">
-        <f>J42/E73*E69</f>
-        <v>4.0731250000000001</v>
-      </c>
-      <c r="M42">
-        <f>LOG10(L42/1000)</f>
-        <v>-2.3900722616603254</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
       <c r="B43" s="9" t="s">
         <v>80</v>
       </c>
@@ -2068,17 +2092,33 @@
         <v>35</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E43" s="15">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="G43">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="J43">
+        <f>E45+E44</f>
+        <v>0.7</v>
+      </c>
+      <c r="K43">
+        <f>LOG10(J43/1000)</f>
+        <v>-3.1549019599857431</v>
+      </c>
+      <c r="L43">
+        <f>J43/E74*E70</f>
+        <v>4.0731250000000001</v>
+      </c>
+      <c r="M43">
+        <f>LOG10(L43/1000)</f>
+        <v>-2.3900722616603254</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="9" t="s">
         <v>80</v>
       </c>
@@ -2086,17 +2126,17 @@
         <v>35</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E44" s="15">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G44">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
+      <c r="A45" s="31"/>
       <c r="B45" s="9" t="s">
         <v>80</v>
       </c>
@@ -2104,37 +2144,37 @@
         <v>35</v>
       </c>
       <c r="D45" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
+      <c r="B46" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E46" s="15">
         <v>0</v>
       </c>
-      <c r="G45">
+      <c r="G46">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="15">
-        <v>10.9</v>
-      </c>
-      <c r="G46">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
       <c r="B47" s="9" t="s">
         <v>80</v>
       </c>
@@ -2142,25 +2182,17 @@
         <v>68</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E47" s="15">
-        <v>6.68</v>
+        <v>10.9</v>
       </c>
       <c r="G47">
-        <v>39</v>
-      </c>
-      <c r="J47">
-        <f>E48+E47</f>
-        <v>16.7</v>
-      </c>
-      <c r="K47">
-        <f>LOG10(J47)</f>
-        <v>1.2227164711475833</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="9" t="s">
         <v>80</v>
       </c>
@@ -2168,17 +2200,25 @@
         <v>68</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E48" s="15">
-        <v>10.02</v>
+        <v>6.68</v>
       </c>
       <c r="G48">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="J48">
+        <f>E49+E48</f>
+        <v>16.7</v>
+      </c>
+      <c r="K48">
+        <f>LOG10(J48)</f>
+        <v>1.2227164711475833</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="9" t="s">
         <v>80</v>
       </c>
@@ -2186,35 +2226,37 @@
         <v>68</v>
       </c>
       <c r="D49" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" s="15">
+        <v>10.02</v>
+      </c>
+      <c r="G49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="31"/>
+      <c r="B50" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E50" s="15">
         <v>18</v>
       </c>
-      <c r="G49">
+      <c r="G50">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="15"/>
-      <c r="F50" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
       <c r="B51" s="9" t="s">
         <v>80</v>
       </c>
@@ -2222,7 +2264,7 @@
         <v>140</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="16" t="s">
@@ -2230,7 +2272,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="31"/>
       <c r="B52" s="9" t="s">
         <v>80</v>
       </c>
@@ -2238,7 +2280,7 @@
         <v>140</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E52" s="15"/>
       <c r="F52" s="16" t="s">
@@ -2246,7 +2288,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="31"/>
       <c r="B53" s="9" t="s">
         <v>80</v>
       </c>
@@ -2254,7 +2296,7 @@
         <v>140</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E53" s="15"/>
       <c r="F53" s="16" t="s">
@@ -2262,41 +2304,25 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
-        <v>144</v>
-      </c>
+      <c r="A54" s="31"/>
       <c r="B54" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E54" s="15"/>
       <c r="F54" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="I54">
-        <f>E69/E70</f>
-        <v>4.6550000000000002</v>
-      </c>
-      <c r="J54">
-        <f>E69/E70</f>
-        <v>4.6550000000000002</v>
-      </c>
-      <c r="K54">
-        <f>LOG10(J54)</f>
-        <v>0.66791968531736146</v>
-      </c>
-      <c r="M54">
-        <f>LOG10((E47+E48)/1000)</f>
-        <v>-1.7772835288524167</v>
-      </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="31" t="s">
+        <v>144</v>
+      </c>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -2304,27 +2330,31 @@
         <v>138</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="16" t="s">
         <v>142</v>
       </c>
+      <c r="I55">
+        <f>E70/E71</f>
+        <v>4.6550000000000002</v>
+      </c>
       <c r="J55">
-        <f>E74/E73</f>
-        <v>0.375</v>
+        <f>E70/E71</f>
+        <v>4.6550000000000002</v>
       </c>
       <c r="K55">
         <f>LOG10(J55)</f>
-        <v>-0.42596873227228116</v>
+        <v>0.66791968531736146</v>
       </c>
       <c r="M55">
-        <f>LOG10((E43+E44)/1000)</f>
-        <v>-3.1549019599857431</v>
+        <f>LOG10((E48+E49)/1000)</f>
+        <v>-1.7772835288524167</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
+      <c r="A56" s="31"/>
       <c r="B56" s="9" t="s">
         <v>80</v>
       </c>
@@ -2332,15 +2362,27 @@
         <v>138</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="16" t="s">
         <v>142</v>
       </c>
+      <c r="J56">
+        <f>E75/E74</f>
+        <v>0.375</v>
+      </c>
+      <c r="K56">
+        <f>LOG10(J56)</f>
+        <v>-0.42596873227228116</v>
+      </c>
+      <c r="M56">
+        <f>LOG10((E44+E45)/1000)</f>
+        <v>-3.1549019599857431</v>
+      </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="31"/>
       <c r="B57" s="9" t="s">
         <v>80</v>
       </c>
@@ -2348,45 +2390,37 @@
         <v>138</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E57" s="15"/>
       <c r="F57" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="J57">
-        <f>(E47+E48)/1000/(E69*PI()/4*E70^2)</f>
-        <v>0.57097476898703581</v>
-      </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="s">
-        <v>145</v>
-      </c>
+      <c r="A58" s="31"/>
       <c r="B58" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E58" s="15"/>
       <c r="F58" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="I58">
-        <f>E69/E74</f>
-        <v>15.516666666666667</v>
-      </c>
       <c r="J58">
-        <f>(E43+E44)/1000/(E73*PI()/4*E74^2)</f>
-        <v>1.5473397245045379</v>
+        <f>(E48+E49)/1000/(E70*PI()/4*E71^2)</f>
+        <v>0.57097476898703581</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="31" t="s">
+        <v>145</v>
+      </c>
       <c r="B59" s="9" t="s">
         <v>80</v>
       </c>
@@ -2394,15 +2428,23 @@
         <v>141</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E59" s="15"/>
       <c r="F59" s="16" t="s">
         <v>142</v>
       </c>
+      <c r="I59">
+        <f>E70/E75</f>
+        <v>15.516666666666667</v>
+      </c>
+      <c r="J59">
+        <f>(E44+E45)/1000/(E74*PI()/4*E75^2)</f>
+        <v>1.5473397245045379</v>
+      </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+      <c r="A60" s="31"/>
       <c r="B60" s="9" t="s">
         <v>80</v>
       </c>
@@ -2410,7 +2452,7 @@
         <v>141</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E60" s="15"/>
       <c r="F60" s="16" t="s">
@@ -2418,7 +2460,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="31"/>
       <c r="B61" s="9" t="s">
         <v>80</v>
       </c>
@@ -2426,41 +2468,41 @@
         <v>141</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E61" s="15"/>
       <c r="F61" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="K61">
-        <f>(K54-K55)/K55</f>
-        <v>-2.5680016741003988</v>
-      </c>
-      <c r="M61">
-        <f>(M55-M54)/M55</f>
-        <v>0.43665966442252035</v>
-      </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="30" t="s">
-        <v>146</v>
-      </c>
+      <c r="A62" s="31"/>
       <c r="B62" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E62" s="15"/>
       <c r="F62" s="16" t="s">
         <v>142</v>
       </c>
+      <c r="K62">
+        <f>(K55-K56)/K56</f>
+        <v>-2.5680016741003988</v>
+      </c>
+      <c r="M62">
+        <f>(M56-M55)/M56</f>
+        <v>0.43665966442252035</v>
+      </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+      <c r="A63" s="31" t="s">
+        <v>146</v>
+      </c>
       <c r="B63" s="9" t="s">
         <v>80</v>
       </c>
@@ -2468,7 +2510,7 @@
         <v>147</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E63" s="15"/>
       <c r="F63" s="16" t="s">
@@ -2476,7 +2518,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
+      <c r="A64" s="31"/>
       <c r="B64" s="9" t="s">
         <v>80</v>
       </c>
@@ -2484,7 +2526,7 @@
         <v>147</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="16" t="s">
@@ -2492,7 +2534,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
+      <c r="A65" s="31"/>
       <c r="B65" s="9" t="s">
         <v>80</v>
       </c>
@@ -2500,462 +2542,460 @@
         <v>147</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="5" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="31"/>
+      <c r="B66" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E66" s="15"/>
+      <c r="F66" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="8"/>
-    </row>
-    <row r="67" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
+      <c r="B67" s="5"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="8"/>
+    </row>
+    <row r="68" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="B67" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D67" s="18"/>
-      <c r="E67" s="15">
-        <v>100</v>
-      </c>
-      <c r="G67">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
-        <v>39</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="15">
-        <v>9</v>
+        <v>100</v>
+      </c>
+      <c r="G68">
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="D69" s="18"/>
       <c r="E69" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D70" s="18"/>
+      <c r="E70" s="15">
         <f>0.91+3*0.007</f>
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="B70" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D70" s="18"/>
-      <c r="E70" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="G70">
-        <v>48</v>
-      </c>
-    </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B71" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D71" s="18"/>
       <c r="E71" s="15">
-        <v>1.45</v>
+        <v>0.2</v>
+      </c>
+      <c r="G71">
+        <v>48</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D72" s="18"/>
       <c r="E72" s="15">
-        <v>0.5</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="19" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B73" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D73" s="18"/>
       <c r="E73" s="15">
-        <v>0.16</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B74" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D74" s="18"/>
       <c r="E74" s="15">
-        <v>0.06</v>
-      </c>
-      <c r="G74">
-        <v>49</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B75" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D75" s="18"/>
       <c r="E75" s="15">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="G75">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="15">
         <v>0.01</v>
       </c>
       <c r="G76">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="15">
-        <v>6.6309999999999997E-3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+      <c r="G77">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C78" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D78" s="19"/>
+      <c r="C78" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78" s="18"/>
       <c r="E78" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F78" t="s">
-        <v>115</v>
-      </c>
-      <c r="G78">
-        <v>53</v>
+        <v>6.6309999999999997E-3</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D79" s="19"/>
       <c r="E79" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F79" t="s">
+        <v>115</v>
+      </c>
+      <c r="G79">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D80" s="19"/>
+      <c r="E80" s="15">
         <v>4</v>
       </c>
-      <c r="F79" s="19" t="s">
+      <c r="F80" s="19" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="5" t="s">
+    <row r="81" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="8"/>
-      <c r="G80">
+      <c r="B81" s="5"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="8"/>
+      <c r="G81">
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
+    <row r="82" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D81" s="18"/>
-      <c r="E81" s="15">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="G81">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
-        <v>113</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>86</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D82" s="18"/>
       <c r="E82" s="15">
-        <v>0.5</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="G82">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>86</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="D83" s="18"/>
       <c r="E83" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G83">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D84" s="18"/>
+      <c r="E84" s="15">
         <f>20*0.2*0.69</f>
         <v>2.76</v>
       </c>
-      <c r="F83" s="8" t="s">
+      <c r="F84" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G83">
+      <c r="G84">
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="5" t="s">
+    <row r="85" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="6"/>
-      <c r="F84" t="s">
+      <c r="B85" s="5"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="6"/>
+      <c r="F85" t="s">
         <v>94</v>
       </c>
-      <c r="G84">
+      <c r="G85">
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="19" t="s">
+    <row r="86" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="19" t="s">
         <v>42</v>
-      </c>
-      <c r="B85" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C85" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D85" s="18"/>
-      <c r="E85" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="F85" t="s">
-        <v>99</v>
-      </c>
-      <c r="G85">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="19" t="s">
-        <v>44</v>
       </c>
       <c r="B86" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D86" s="18"/>
       <c r="E86" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F86" t="s">
+        <v>99</v>
+      </c>
+      <c r="G86">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B87" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D87" s="18"/>
+      <c r="E87" s="15">
         <v>365</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F87" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="5" t="s">
+    <row r="88" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B87" s="5"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="7"/>
-      <c r="E87" s="6"/>
-      <c r="G87">
+      <c r="B88" s="5"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="6"/>
+      <c r="G88">
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="19" t="s">
+    <row r="89" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="B88" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D88" s="18">
-        <v>1</v>
-      </c>
-      <c r="E88" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G88">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="19" t="s">
-        <v>50</v>
       </c>
       <c r="B89" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D89" s="18">
         <v>1</v>
       </c>
-      <c r="E89" s="15">
-        <v>207</v>
+      <c r="E89" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="G89">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="B90" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D90" s="18">
         <v>1</v>
       </c>
-      <c r="E90" s="12" t="s">
-        <v>97</v>
+      <c r="E90" s="15">
+        <v>207</v>
       </c>
       <c r="G90">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D91" s="18">
         <v>1</v>
       </c>
-      <c r="E91">
-        <v>20</v>
+      <c r="E91" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G91">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="19"/>
+      <c r="A92" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="B92" s="19" t="s">
         <v>87</v>
       </c>
@@ -2965,11 +3005,11 @@
       <c r="D92" s="18">
         <v>1</v>
       </c>
-      <c r="E92" s="15">
-        <v>30</v>
+      <c r="E92">
+        <v>20</v>
       </c>
       <c r="G92">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -2984,10 +3024,10 @@
         <v>1</v>
       </c>
       <c r="E93" s="15">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="G93">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3002,10 +3042,10 @@
         <v>1</v>
       </c>
       <c r="E94" s="15">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G94">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3019,34 +3059,32 @@
       <c r="D95" s="18">
         <v>1</v>
       </c>
-      <c r="E95" s="15"/>
+      <c r="E95" s="15">
+        <v>100</v>
+      </c>
       <c r="G95">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="19" t="s">
-        <v>101</v>
-      </c>
+      <c r="A96" s="19"/>
       <c r="B96" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D96" s="18">
         <v>1</v>
       </c>
-      <c r="E96" s="15">
-        <v>0</v>
-      </c>
+      <c r="E96" s="15"/>
       <c r="G96">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B97" s="19" t="s">
         <v>87</v>
@@ -3058,15 +3096,15 @@
         <v>1</v>
       </c>
       <c r="E97" s="15">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G97">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B98" s="19" t="s">
         <v>87</v>
@@ -3078,14 +3116,16 @@
         <v>1</v>
       </c>
       <c r="E98" s="15">
-        <v>0.67</v>
+        <v>0.01</v>
       </c>
       <c r="G98">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="19"/>
+      <c r="A99" s="19" t="s">
+        <v>103</v>
+      </c>
       <c r="B99" s="19" t="s">
         <v>87</v>
       </c>
@@ -3096,7 +3136,10 @@
         <v>1</v>
       </c>
       <c r="E99" s="15">
-        <v>1</v>
+        <v>0.67</v>
+      </c>
+      <c r="G99">
+        <v>76</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3110,93 +3153,90 @@
       <c r="D100" s="18">
         <v>1</v>
       </c>
-      <c r="E100" s="15"/>
-      <c r="G100">
-        <v>77</v>
+      <c r="E100" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="19" t="s">
-        <v>53</v>
-      </c>
+      <c r="A101" s="19"/>
       <c r="B101" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C101" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D101" s="18">
+        <v>1</v>
+      </c>
+      <c r="E101" s="15"/>
+      <c r="G101">
         <v>77</v>
-      </c>
-      <c r="D101" s="18">
-        <v>2</v>
-      </c>
-      <c r="E101" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G101">
-        <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B102" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D102" s="18">
         <v>2</v>
       </c>
-      <c r="E102" s="15">
-        <v>365</v>
+      <c r="E102" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="G102">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="19" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="B103" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D103" s="18">
         <v>2</v>
       </c>
-      <c r="E103" s="12" t="s">
-        <v>97</v>
+      <c r="E103" s="15">
+        <v>365</v>
       </c>
       <c r="G103">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="19" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B104" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D104" s="18">
         <v>2</v>
       </c>
-      <c r="E104" s="15">
-        <v>0</v>
+      <c r="E104" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G104">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="19"/>
+      <c r="A105" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="B105" s="19" t="s">
         <v>87</v>
       </c>
@@ -3207,10 +3247,10 @@
         <v>2</v>
       </c>
       <c r="E105" s="15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G105">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3225,10 +3265,10 @@
         <v>2</v>
       </c>
       <c r="E106" s="15">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G106">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3243,10 +3283,10 @@
         <v>2</v>
       </c>
       <c r="E107" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="G107">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3261,35 +3301,33 @@
         <v>2</v>
       </c>
       <c r="E108" s="15">
-        <v>1.69</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G108">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="19" t="s">
-        <v>56</v>
-      </c>
+      <c r="A109" s="19"/>
       <c r="B109" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D109" s="18">
         <v>2</v>
       </c>
       <c r="E109" s="15">
-        <v>0</v>
+        <v>1.69</v>
       </c>
       <c r="G109">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="19" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="B110" s="19" t="s">
         <v>87</v>
@@ -3303,10 +3341,13 @@
       <c r="E110" s="15">
         <v>0</v>
       </c>
+      <c r="G110">
+        <v>86</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B111" s="19" t="s">
         <v>87</v>
@@ -3318,11 +3359,13 @@
         <v>2</v>
       </c>
       <c r="E111" s="15">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="19"/>
+      <c r="A112" s="19" t="s">
+        <v>103</v>
+      </c>
       <c r="B112" s="19" t="s">
         <v>87</v>
       </c>
@@ -3333,7 +3376,7 @@
         <v>2</v>
       </c>
       <c r="E112" s="15">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,10 +3395,19 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="20"/>
-      <c r="B114" s="20"/>
-      <c r="C114" s="21"/>
-      <c r="D114" s="22"/>
+      <c r="A114" s="19"/>
+      <c r="B114" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D114" s="18">
+        <v>2</v>
+      </c>
+      <c r="E114" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="20"/>
@@ -4013,6 +4065,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="20"/>
+      <c r="B224" s="20"/>
       <c r="C224" s="21"/>
       <c r="D224" s="22"/>
     </row>
@@ -4061,17 +4114,22 @@
       <c r="C233" s="21"/>
       <c r="D233" s="22"/>
     </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="20"/>
+      <c r="C234" s="21"/>
+      <c r="D234" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A43:A45"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="18">
@@ -4084,10 +4142,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{FCAB33B4-E22D-416A-9EE8-1B6629F4B7A9}">
       <formula1>"angiosperm, gymnosperm"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E86" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E87" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E87 E82 E84:E85" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E88 E83 E85:E86" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4098,7 +4156,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{5620C1FF-B28B-4556-ADEF-5FA98FE67CB9}">
       <formula1>"C3, C4, CAM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E35 E19 E26" xr:uid="{D43B937F-2CE8-47D9-A978-7D336015DF11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E36 E19 E27" xr:uid="{D43B937F-2CE8-47D9-A978-7D336015DF11}">
       <formula1>"Annual, Herbaceous perennial, Woody perennial"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{6E5E4A37-6A5B-480B-8E8F-63973FC4A36F}">
@@ -4113,7 +4171,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{793E17DF-C558-4DAF-B608-9E20297CD619}">
       <formula1>"annual, perennial evergreen, perennial deciduous"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E90 E103" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E91 E104" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E20" xr:uid="{DC451139-D175-47A3-922A-D7E1D89FD320}">
@@ -4144,10 +4202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
-  <dimension ref="A1:N233"/>
+  <dimension ref="A1:N234"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4492,7 +4550,7 @@
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="15">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="G20" t="s">
         <v>166</v>
@@ -4536,7 +4594,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="15">
@@ -4566,48 +4624,45 @@
         <v>162</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="15">
         <v>120</v>
       </c>
-      <c r="G25" t="s">
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G26" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G27">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
       <c r="B28" s="9" t="s">
         <v>80</v>
       </c>
@@ -4615,17 +4670,17 @@
         <v>58</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E28" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G28">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="9" t="s">
         <v>80</v>
       </c>
@@ -4633,17 +4688,17 @@
         <v>58</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E29" s="15">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G29">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="9" t="s">
         <v>80</v>
       </c>
@@ -4651,37 +4706,37 @@
         <v>58</v>
       </c>
       <c r="D30" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="G30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E31" s="15">
         <v>0.01</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" s="15">
-        <v>1.444</v>
-      </c>
-      <c r="G31">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
       <c r="B32" s="9" t="s">
         <v>80</v>
       </c>
@@ -4689,17 +4744,17 @@
         <v>27</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E32" s="15">
-        <v>1.5129999999999999</v>
+        <v>1.444</v>
       </c>
       <c r="G32">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="A33" s="33"/>
       <c r="B33" s="9" t="s">
         <v>80</v>
       </c>
@@ -4707,17 +4762,17 @@
         <v>27</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E33" s="15">
-        <v>1.4630000000000001</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="G33">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="9" t="s">
         <v>80</v>
       </c>
@@ -4725,51 +4780,47 @@
         <v>27</v>
       </c>
       <c r="D34" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="15">
+        <v>1.4630000000000001</v>
+      </c>
+      <c r="G34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E35" s="15">
         <v>1.4139999999999999</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:14" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:14" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="G36">
-        <v>27</v>
-      </c>
-      <c r="H36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
       <c r="B37" s="9" t="s">
         <v>80</v>
       </c>
@@ -4777,16 +4828,21 @@
         <v>88</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E37" s="15"/>
-      <c r="F37" s="34"/>
+      <c r="F37" s="35" t="s">
+        <v>90</v>
+      </c>
       <c r="G37">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="H37" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="9" t="s">
         <v>80</v>
       </c>
@@ -4794,33 +4850,33 @@
         <v>88</v>
       </c>
       <c r="D38" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="F38" s="35"/>
+      <c r="G38">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
+      <c r="B39" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="34"/>
-      <c r="G38">
+      <c r="E39" s="15"/>
+      <c r="F39" s="35"/>
+      <c r="G39">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" s="15"/>
-      <c r="F39" s="34"/>
-      <c r="G39">
-        <v>30</v>
-      </c>
-    </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="9" t="s">
         <v>80</v>
       </c>
@@ -4828,16 +4884,16 @@
         <v>89</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E40" s="15"/>
-      <c r="F40" s="34"/>
+      <c r="F40" s="35"/>
       <c r="G40">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="9" t="s">
         <v>80</v>
       </c>
@@ -4845,36 +4901,35 @@
         <v>89</v>
       </c>
       <c r="D41" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="35"/>
+      <c r="G41">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
+      <c r="B42" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="34"/>
-      <c r="G41">
+      <c r="E42" s="15"/>
+      <c r="F42" s="35"/>
+      <c r="G42">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="G42">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
       <c r="B43" s="9" t="s">
         <v>80</v>
       </c>
@@ -4882,18 +4937,17 @@
         <v>35</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="27">
-        <f>E44/0.27*0.2</f>
-        <v>2.2222222222222223E-2</v>
+        <v>91</v>
+      </c>
+      <c r="E43" s="15">
+        <v>0.01</v>
       </c>
       <c r="G43">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="9" t="s">
         <v>80</v>
       </c>
@@ -4901,17 +4955,18 @@
         <v>35</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="15">
-        <v>0.03</v>
+        <v>92</v>
+      </c>
+      <c r="E44" s="27">
+        <f>E45/0.27*0.2</f>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="G44">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+      <c r="A45" s="31"/>
       <c r="B45" s="9" t="s">
         <v>80</v>
       </c>
@@ -4919,37 +4974,37 @@
         <v>35</v>
       </c>
       <c r="D45" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="G45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="31"/>
+      <c r="B46" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E46" s="15">
         <v>0</v>
       </c>
-      <c r="G45">
+      <c r="G46">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="15">
-        <v>4.3</v>
-      </c>
-      <c r="G46">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
       <c r="B47" s="9" t="s">
         <v>80</v>
       </c>
@@ -4957,33 +5012,17 @@
         <v>68</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E47" s="15">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="G47">
-        <v>39</v>
-      </c>
-      <c r="J47">
-        <f>E47+E48</f>
-        <v>9.6</v>
-      </c>
-      <c r="K47">
-        <f>LOG10(J47/1000)</f>
-        <v>-2.0177287669604316</v>
-      </c>
-      <c r="M47">
-        <f>E69/E70</f>
-        <v>2.5</v>
-      </c>
-      <c r="N47">
-        <f>LOG10(M47)</f>
-        <v>0.3979400086720376</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="9" t="s">
         <v>80</v>
       </c>
@@ -4991,33 +5030,33 @@
         <v>68</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E48" s="15">
-        <v>5.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G48">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J48">
-        <f>(E43+E44)/E73*E69</f>
-        <v>0.52222222222222237</v>
+        <f>E48+E49</f>
+        <v>9.6</v>
       </c>
       <c r="K48">
         <f>LOG10(J48/1000)</f>
-        <v>-3.2821446515036072</v>
+        <v>-2.0177287669604316</v>
       </c>
       <c r="M48">
-        <f>E69/E74</f>
-        <v>138.2930051648863</v>
+        <f>E70/E71</f>
+        <v>2.5</v>
       </c>
       <c r="N48">
         <f>LOG10(M48)</f>
-        <v>2.1408002141287135</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+        <v>0.3979400086720376</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="31"/>
       <c r="B49" s="9" t="s">
         <v>80</v>
       </c>
@@ -5025,35 +5064,53 @@
         <v>68</v>
       </c>
       <c r="D49" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="G49">
+        <v>40</v>
+      </c>
+      <c r="J49">
+        <f>(E44+E45)/E74*E70</f>
+        <v>0.52222222222222237</v>
+      </c>
+      <c r="K49">
+        <f>LOG10(J49/1000)</f>
+        <v>-3.2821446515036072</v>
+      </c>
+      <c r="M49">
+        <f>E70/E75</f>
+        <v>138.2930051648863</v>
+      </c>
+      <c r="N49">
+        <f>LOG10(M49)</f>
+        <v>2.1408002141287135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="31"/>
+      <c r="B50" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E50" s="15">
         <v>4</v>
       </c>
-      <c r="G49">
+      <c r="G50">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="15"/>
-      <c r="F50" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
       <c r="B51" s="9" t="s">
         <v>80</v>
       </c>
@@ -5061,15 +5118,15 @@
         <v>140</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="31"/>
       <c r="B52" s="9" t="s">
         <v>80</v>
       </c>
@@ -5077,15 +5134,15 @@
         <v>140</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E52" s="15"/>
       <c r="F52" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
       <c r="B53" s="9" t="s">
         <v>80</v>
       </c>
@@ -5093,33 +5150,33 @@
         <v>140</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E53" s="15"/>
       <c r="F53" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
-        <v>144</v>
-      </c>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="31"/>
       <c r="B54" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E54" s="15"/>
       <c r="F54" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="31" t="s">
+        <v>144</v>
+      </c>
       <c r="B55" s="9" t="s">
         <v>80</v>
       </c>
@@ -5127,15 +5184,15 @@
         <v>138</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="31"/>
       <c r="B56" s="9" t="s">
         <v>80</v>
       </c>
@@ -5143,15 +5200,15 @@
         <v>138</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="31"/>
       <c r="B57" s="9" t="s">
         <v>80</v>
       </c>
@@ -5159,33 +5216,33 @@
         <v>138</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E57" s="15"/>
       <c r="F57" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="s">
-        <v>145</v>
-      </c>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
       <c r="B58" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E58" s="15"/>
       <c r="F58" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="31" t="s">
+        <v>145</v>
+      </c>
       <c r="B59" s="9" t="s">
         <v>80</v>
       </c>
@@ -5193,15 +5250,15 @@
         <v>141</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E59" s="15"/>
       <c r="F59" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="31"/>
       <c r="B60" s="9" t="s">
         <v>80</v>
       </c>
@@ -5209,15 +5266,15 @@
         <v>141</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E60" s="15"/>
       <c r="F60" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="31"/>
       <c r="B61" s="9" t="s">
         <v>80</v>
       </c>
@@ -5225,33 +5282,33 @@
         <v>141</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E61" s="15"/>
       <c r="F61" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="30" t="s">
-        <v>146</v>
-      </c>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="31"/>
       <c r="B62" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E62" s="15"/>
       <c r="F62" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="31" t="s">
+        <v>146</v>
+      </c>
       <c r="B63" s="9" t="s">
         <v>80</v>
       </c>
@@ -5259,15 +5316,15 @@
         <v>147</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E63" s="15"/>
       <c r="F63" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
       <c r="B64" s="9" t="s">
         <v>80</v>
       </c>
@@ -5275,7 +5332,7 @@
         <v>147</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="16" t="s">
@@ -5283,7 +5340,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
+      <c r="A65" s="31"/>
       <c r="B65" s="9" t="s">
         <v>80</v>
       </c>
@@ -5291,478 +5348,476 @@
         <v>147</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="5" t="s">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="31"/>
+      <c r="B66" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E66" s="15"/>
+      <c r="F66" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="8"/>
-      <c r="J66">
-        <f>PI()/4*E70^2*E69</f>
+      <c r="B67" s="5"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="8"/>
+      <c r="J67">
+        <f>PI()/4*E71^2*E70</f>
         <v>5.3014376029327764E-2</v>
       </c>
-      <c r="K66">
-        <f>J47/1000/J66</f>
+      <c r="K67">
+        <f>J48/1000/J67</f>
         <v>0.18108295747344533</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
+    <row r="68" spans="1:13" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="B67" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D67" s="18"/>
-      <c r="E67" s="15">
-        <v>18</v>
-      </c>
-      <c r="I67">
-        <f>E69/E74</f>
-        <v>138.2930051648863</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
-        <v>39</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="15">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="I68">
-        <f>E69/E70</f>
-        <v>2.5</v>
+        <f>E70/E75</f>
+        <v>138.2930051648863</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="D69" s="18"/>
       <c r="E69" s="15">
-        <v>0.75</v>
+        <v>10</v>
+      </c>
+      <c r="I69">
+        <f>E70/E71</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="D70" s="18"/>
       <c r="E70" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="G70">
-        <v>48</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B71" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D71" s="18"/>
       <c r="E71" s="15">
-        <v>0.33</v>
+        <v>0.3</v>
+      </c>
+      <c r="G71">
+        <v>48</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D72" s="18"/>
       <c r="E72" s="15">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="19" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B73" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D73" s="18"/>
       <c r="E73" s="15">
-        <f>E69/10</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="K73" t="e">
-        <f>(K66-K67)/K67</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M73" t="e">
-        <f>(M67-M66)/M67</f>
-        <v>#DIV/0!</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B74" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C74" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D74" s="18"/>
+      <c r="E74" s="15">
+        <f>E70/10</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K74" t="e">
+        <f>(K67-K68)/K68</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M74" t="e">
+        <f>(M68-M67)/M68</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="27">
+      <c r="D75" s="18"/>
+      <c r="E75" s="27">
         <f>SQRT(0.231/100/100*4/PI())</f>
         <v>5.423267786434878E-3</v>
       </c>
-      <c r="G74">
+      <c r="G75">
         <v>49</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B75" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="15">
-        <v>0.02</v>
-      </c>
-      <c r="G75">
-        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="15">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G76">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="15">
-        <v>7.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+      <c r="G77">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C78" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D78" s="19"/>
+      <c r="C78" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78" s="18"/>
       <c r="E78" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F78" t="s">
-        <v>115</v>
-      </c>
-      <c r="G78">
-        <v>53</v>
+        <v>7.4000000000000003E-3</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D79" s="19"/>
       <c r="E79" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F79" t="s">
+        <v>115</v>
+      </c>
+      <c r="G79">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D80" s="19"/>
+      <c r="E80" s="15">
         <v>4</v>
       </c>
-      <c r="F79" s="19" t="s">
+      <c r="F80" s="19" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="5" t="s">
+    <row r="81" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="8"/>
-      <c r="G80">
+      <c r="B81" s="5"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="8"/>
+      <c r="G81">
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
+    <row r="82" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D81" s="18"/>
-      <c r="E81" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="G81">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
-        <v>113</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>86</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D82" s="18"/>
       <c r="E82" s="15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G82">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>86</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="D83" s="18"/>
       <c r="E83" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G83">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D84" s="18"/>
+      <c r="E84" s="15">
         <v>1.2</v>
       </c>
-      <c r="G83">
+      <c r="G84">
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="5" t="s">
+    <row r="85" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="8" t="s">
+      <c r="B85" s="5"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G84">
+      <c r="G85">
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="19" t="s">
+    <row r="86" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="19" t="s">
         <v>42</v>
-      </c>
-      <c r="B85" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C85" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D85" s="18"/>
-      <c r="E85" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="G85">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="19" t="s">
-        <v>44</v>
       </c>
       <c r="B86" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D86" s="18"/>
       <c r="E86" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G86">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B87" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D87" s="18"/>
+      <c r="E87" s="15">
         <v>365</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F87" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="5" t="s">
+    <row r="88" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B87" s="5"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="7"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="8"/>
-      <c r="G87">
+      <c r="B88" s="5"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="8"/>
+      <c r="G88">
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="19" t="s">
+    <row r="89" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="B88" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D88" s="18">
-        <v>1</v>
-      </c>
-      <c r="E88" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G88">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="19" t="s">
-        <v>50</v>
       </c>
       <c r="B89" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D89" s="18">
         <v>1</v>
       </c>
-      <c r="E89" s="15">
-        <v>207</v>
+      <c r="E89" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="G89">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="B90" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D90" s="18">
         <v>1</v>
       </c>
-      <c r="E90" s="12" t="s">
-        <v>97</v>
+      <c r="E90" s="15">
+        <v>207</v>
       </c>
       <c r="G90">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D91" s="18">
         <v>1</v>
       </c>
-      <c r="E91" s="15">
-        <v>30</v>
+      <c r="E91" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G91">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="19"/>
+      <c r="A92" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="B92" s="19" t="s">
         <v>87</v>
       </c>
@@ -5773,10 +5828,10 @@
         <v>1</v>
       </c>
       <c r="E92" s="15">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G92">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -5791,10 +5846,10 @@
         <v>1</v>
       </c>
       <c r="E93" s="15">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G93">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -5809,10 +5864,10 @@
         <v>1</v>
       </c>
       <c r="E94" s="15">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G94">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -5826,33 +5881,33 @@
       <c r="D95" s="18">
         <v>1</v>
       </c>
-      <c r="E95" s="15"/>
+      <c r="E95" s="15">
+        <v>55</v>
+      </c>
       <c r="G95">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="19" t="s">
-        <v>52</v>
-      </c>
+      <c r="A96" s="19"/>
       <c r="B96" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D96" s="18">
         <v>1</v>
       </c>
-      <c r="E96" s="15">
-        <v>0.01</v>
-      </c>
+      <c r="E96" s="15"/>
       <c r="G96">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="19"/>
+      <c r="A97" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="B97" s="19" t="s">
         <v>87</v>
       </c>
@@ -5863,10 +5918,10 @@
         <v>1</v>
       </c>
       <c r="E97" s="15">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="G97">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -5881,10 +5936,10 @@
         <v>1</v>
       </c>
       <c r="E98" s="15">
-        <v>0.67</v>
+        <v>0.25</v>
       </c>
       <c r="G98">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -5899,10 +5954,10 @@
         <v>1</v>
       </c>
       <c r="E99" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="F99" t="s">
-        <v>100</v>
+        <v>0.67</v>
+      </c>
+      <c r="G99">
+        <v>76</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -5916,93 +5971,93 @@
       <c r="D100" s="18">
         <v>1</v>
       </c>
-      <c r="E100" s="15"/>
-      <c r="G100">
-        <v>77</v>
+      <c r="E100" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F100" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="19" t="s">
-        <v>53</v>
-      </c>
+      <c r="A101" s="19"/>
       <c r="B101" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C101" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D101" s="18">
+        <v>1</v>
+      </c>
+      <c r="E101" s="15"/>
+      <c r="G101">
         <v>77</v>
-      </c>
-      <c r="D101" s="18">
-        <v>2</v>
-      </c>
-      <c r="E101" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G101">
-        <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B102" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D102" s="18">
         <v>2</v>
       </c>
-      <c r="E102" s="15">
-        <v>365</v>
+      <c r="E102" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="G102">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="19" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="B103" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D103" s="18">
         <v>2</v>
       </c>
-      <c r="E103" s="12" t="s">
-        <v>97</v>
+      <c r="E103" s="15">
+        <v>365</v>
       </c>
       <c r="G103">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="19" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="B104" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D104" s="18">
         <v>2</v>
       </c>
-      <c r="E104" s="15">
-        <v>0</v>
+      <c r="E104" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G104">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="19"/>
+      <c r="A105" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="B105" s="19" t="s">
         <v>87</v>
       </c>
@@ -6013,10 +6068,10 @@
         <v>2</v>
       </c>
       <c r="E105" s="15">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G105">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -6031,10 +6086,10 @@
         <v>2</v>
       </c>
       <c r="E106" s="15">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G106">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -6049,10 +6104,10 @@
         <v>2</v>
       </c>
       <c r="E107" s="15">
-        <v>0.68</v>
+        <v>0.6</v>
       </c>
       <c r="G107">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -6067,34 +6122,34 @@
         <v>2</v>
       </c>
       <c r="E108" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="G108">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="19" t="s">
-        <v>56</v>
-      </c>
+      <c r="A109" s="19"/>
       <c r="B109" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D109" s="18">
         <v>2</v>
       </c>
       <c r="E109" s="15">
-        <v>0</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G109">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="19"/>
+      <c r="A110" s="19" t="s">
+        <v>56</v>
+      </c>
       <c r="B110" s="19" t="s">
         <v>87</v>
       </c>
@@ -6106,6 +6161,9 @@
       </c>
       <c r="E110" s="15">
         <v>0</v>
+      </c>
+      <c r="G110">
+        <v>86</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -6120,7 +6178,7 @@
         <v>2</v>
       </c>
       <c r="E111" s="15">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -6135,7 +6193,7 @@
         <v>2</v>
       </c>
       <c r="E112" s="15">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -6154,10 +6212,19 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="20"/>
-      <c r="B114" s="20"/>
-      <c r="C114" s="21"/>
-      <c r="D114" s="22"/>
+      <c r="A114" s="19"/>
+      <c r="B114" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D114" s="18">
+        <v>2</v>
+      </c>
+      <c r="E114" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="20"/>
@@ -6873,21 +6940,27 @@
       <c r="C233" s="21"/>
       <c r="D233" s="22"/>
     </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="20"/>
+      <c r="B234" s="20"/>
+      <c r="C234" s="21"/>
+      <c r="D234" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="F36:F41"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A43:A46"/>
   </mergeCells>
   <dataValidations count="18">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E35 E19" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E36 E19" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
       <formula1>"Annual, Herbaceous perennial, Woody perennial"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{BF09F0A8-DEDC-4564-B7AE-B6347D314DF5}">
@@ -6897,11 +6970,11 @@
       <formula1>1</formula1>
       <formula2>366</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E87 E82 E84:E85" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E88 E83 E85:E86" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E86" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E87" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{9966BE53-3AF7-47D9-9DC3-79C6924CF42E}">
@@ -6925,10 +6998,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9" xr:uid="{82D88EBD-3D9A-4158-A9B3-F883994282C6}">
       <formula1>"climbing,columnar,conical,decumbent,erect,irregular,oval,prostrate,rounded,semi_erect,vase"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E90 E103" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E91 E104" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E20 E26" xr:uid="{CC49B6F4-DDA3-41C3-9192-398A844CBA5C}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E20 E27" xr:uid="{CC49B6F4-DDA3-41C3-9192-398A844CBA5C}">
       <formula1>0</formula1>
       <formula2>250</formula2>
     </dataValidation>
@@ -6940,13 +7013,13 @@
       <formula1>0</formula1>
       <formula2>800000</formula2>
     </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23" xr:uid="{036093C0-53D0-4F98-9007-9733283CE490}">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24:E25" xr:uid="{C087BDC9-F4AC-4DFE-80A9-3E8AE2633514}">
       <formula1>0</formula1>
       <formula2>900000</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23" xr:uid="{036093C0-53D0-4F98-9007-9733283CE490}">
-      <formula1>0</formula1>
-      <formula2>1000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Editing default plant array for testing
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92704FB-6B8B-4CFA-82DD-2A241E82FFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D59E385-E92A-4649-B80E-F82739E15253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="BTS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2808,7 +2807,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>112</v>
       </c>
@@ -4204,8 +4203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
   <dimension ref="A1:N234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6948,6 +6947,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A43:A46"/>
     <mergeCell ref="A63:A66"/>
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="A55:A58"/>
@@ -6955,9 +6957,6 @@
     <mergeCell ref="F37:F42"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A43:A46"/>
   </mergeCells>
   <dataValidations count="18">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E36 E19" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">

</xml_diff>

<commit_message>
Updated plant array preallocation and passing unit test on plant count
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D59E385-E92A-4649-B80E-F82739E15253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C83A994-83AD-45FE-B27F-5150558C4636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="181">
   <si>
     <t>Parameter</t>
   </si>
@@ -777,6 +777,18 @@
       </rPr>
       <t xml:space="preserve"> concentration</t>
     </r>
+  </si>
+  <si>
+    <t>Maximum basal diameter (m)</t>
+  </si>
+  <si>
+    <t>max_basal_dia</t>
+  </si>
+  <si>
+    <t>Minimum basal diameter (m)</t>
+  </si>
+  <si>
+    <t>min_basal_dia</t>
   </si>
 </sst>
 </file>
@@ -1358,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
-  <dimension ref="A1:M234"/>
+  <dimension ref="A1:M236"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,7 +2120,7 @@
         <v>-3.1549019599857431</v>
       </c>
       <c r="L43">
-        <f>J43/E74*E70</f>
+        <f>J43/E75*E70</f>
         <v>4.0731250000000001</v>
       </c>
       <c r="M43">
@@ -2368,7 +2380,7 @@
         <v>142</v>
       </c>
       <c r="J56">
-        <f>E75/E74</f>
+        <f>E76/E75</f>
         <v>0.375</v>
       </c>
       <c r="K56">
@@ -2434,11 +2446,11 @@
         <v>142</v>
       </c>
       <c r="I59">
-        <f>E70/E75</f>
+        <f>E70/E76</f>
         <v>15.516666666666667</v>
       </c>
       <c r="J59">
-        <f>(E44+E45)/1000/(E74*PI()/4*E75^2)</f>
+        <f>(E44+E45)/1000/(E75*PI()/4*E76^2)</f>
         <v>1.5473397245045379</v>
       </c>
     </row>
@@ -2673,364 +2685,354 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
-        <v>119</v>
+        <v>177</v>
       </c>
       <c r="B74" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
       <c r="D74" s="18"/>
-      <c r="E74" s="15">
-        <v>0.16</v>
-      </c>
+      <c r="E74" s="15"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B75" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D75" s="18"/>
       <c r="E75" s="15">
-        <v>0.06</v>
-      </c>
-      <c r="G75">
-        <v>49</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="15">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="G76">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>125</v>
+        <v>180</v>
       </c>
       <c r="D77" s="18"/>
-      <c r="E77" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="G77">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E77" s="15"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D78" s="18"/>
       <c r="E78" s="15">
-        <v>6.6309999999999997E-3</v>
+        <v>0.01</v>
+      </c>
+      <c r="G78">
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C79" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D79" s="19"/>
+      <c r="C79" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D79" s="18"/>
       <c r="E79" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F79" t="s">
-        <v>115</v>
+        <v>0.01</v>
       </c>
       <c r="G79">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="18"/>
+      <c r="E80" s="15">
+        <v>6.6309999999999997E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D81" s="19"/>
+      <c r="E81" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F81" t="s">
+        <v>115</v>
+      </c>
+      <c r="G81">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="D80" s="19"/>
-      <c r="E80" s="15">
+      <c r="D82" s="19"/>
+      <c r="E82" s="15">
         <v>4</v>
       </c>
-      <c r="F80" s="19" t="s">
+      <c r="F82" s="19" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+    <row r="83" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="8"/>
-      <c r="G81">
+      <c r="B83" s="5"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="8"/>
+      <c r="G83">
         <v>54</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+    <row r="84" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D82" s="18"/>
-      <c r="E82" s="15">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="G82">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="B83" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D83" s="18"/>
-      <c r="E83" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G83">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="19" t="s">
-        <v>114</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>86</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D84" s="18"/>
       <c r="E84" s="15">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="G84">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B85" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D85" s="18"/>
+      <c r="E85" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G85">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D86" s="18"/>
+      <c r="E86" s="15">
         <f>20*0.2*0.69</f>
         <v>2.76</v>
       </c>
-      <c r="F84" s="8" t="s">
+      <c r="F86" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G84">
+      <c r="G86">
         <v>57</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="5" t="s">
+    <row r="87" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="6"/>
-      <c r="F85" t="s">
+      <c r="B87" s="5"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="6"/>
+      <c r="F87" t="s">
         <v>94</v>
       </c>
-      <c r="G85">
+      <c r="G87">
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="19" t="s">
+    <row r="88" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="B88" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C86" s="17" t="s">
+      <c r="C88" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D86" s="18"/>
-      <c r="E86" s="15">
+      <c r="D88" s="18"/>
+      <c r="E88" s="15">
         <v>0.01</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F88" t="s">
         <v>99</v>
       </c>
-      <c r="G86">
+      <c r="G88">
         <v>59</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="19" t="s">
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B87" s="19" t="s">
+      <c r="B89" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="C89" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D87" s="18"/>
-      <c r="E87" s="15">
+      <c r="D89" s="18"/>
+      <c r="E89" s="15">
         <v>365</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F89" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="5" t="s">
+    <row r="90" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="6"/>
-      <c r="G88">
+      <c r="B90" s="5"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="6"/>
+      <c r="G90">
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="19" t="s">
+    <row r="91" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="B89" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D89" s="18">
-        <v>1</v>
-      </c>
-      <c r="E89" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G89">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D90" s="18">
-        <v>1</v>
-      </c>
-      <c r="E90" s="15">
-        <v>207</v>
-      </c>
-      <c r="G90">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="19" t="s">
-        <v>95</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D91" s="18">
         <v>1</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="G91">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B92" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D92" s="18">
         <v>1</v>
       </c>
-      <c r="E92">
-        <v>20</v>
+      <c r="E92" s="15">
+        <v>207</v>
       </c>
       <c r="G92">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="19"/>
+      <c r="A93" s="19" t="s">
+        <v>95</v>
+      </c>
       <c r="B93" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D93" s="18">
         <v>1</v>
       </c>
-      <c r="E93" s="15">
-        <v>30</v>
+      <c r="E93" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G93">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="19"/>
+      <c r="A94" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="B94" s="19" t="s">
         <v>87</v>
       </c>
@@ -3040,11 +3042,11 @@
       <c r="D94" s="18">
         <v>1</v>
       </c>
-      <c r="E94" s="15">
-        <v>70</v>
+      <c r="E94">
+        <v>20</v>
       </c>
       <c r="G94">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3059,10 +3061,10 @@
         <v>1</v>
       </c>
       <c r="E95" s="15">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="G95">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3076,54 +3078,50 @@
       <c r="D96" s="18">
         <v>1</v>
       </c>
-      <c r="E96" s="15"/>
+      <c r="E96" s="15">
+        <v>70</v>
+      </c>
       <c r="G96">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="19" t="s">
-        <v>101</v>
-      </c>
+      <c r="A97" s="19"/>
       <c r="B97" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D97" s="18">
         <v>1</v>
       </c>
       <c r="E97" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G97">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="19" t="s">
-        <v>102</v>
-      </c>
+      <c r="A98" s="19"/>
       <c r="B98" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D98" s="18">
         <v>1</v>
       </c>
-      <c r="E98" s="15">
-        <v>0.01</v>
-      </c>
+      <c r="E98" s="15"/>
       <c r="G98">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B99" s="19" t="s">
         <v>87</v>
@@ -3135,14 +3133,16 @@
         <v>1</v>
       </c>
       <c r="E99" s="15">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="G99">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="19"/>
+      <c r="A100" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="B100" s="19" t="s">
         <v>87</v>
       </c>
@@ -3153,11 +3153,16 @@
         <v>1</v>
       </c>
       <c r="E100" s="15">
-        <v>1</v>
+        <v>0.01</v>
+      </c>
+      <c r="G100">
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="19"/>
+      <c r="A101" s="19" t="s">
+        <v>103</v>
+      </c>
       <c r="B101" s="19" t="s">
         <v>87</v>
       </c>
@@ -3167,111 +3172,108 @@
       <c r="D101" s="18">
         <v>1</v>
       </c>
-      <c r="E101" s="15"/>
+      <c r="E101" s="15">
+        <v>0.67</v>
+      </c>
       <c r="G101">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="19" t="s">
-        <v>53</v>
-      </c>
+      <c r="A102" s="19"/>
       <c r="B102" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D102" s="18">
-        <v>2</v>
-      </c>
-      <c r="E102" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G102">
-        <v>78</v>
+        <v>1</v>
+      </c>
+      <c r="E102" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="19" t="s">
-        <v>54</v>
-      </c>
+      <c r="A103" s="19"/>
       <c r="B103" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D103" s="18">
-        <v>2</v>
-      </c>
-      <c r="E103" s="15">
-        <v>365</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E103" s="15"/>
       <c r="G103">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="19" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="B104" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D104" s="18">
         <v>2</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="G104">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B105" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D105" s="18">
         <v>2</v>
       </c>
       <c r="E105" s="15">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G105">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="19"/>
+      <c r="A106" s="19" t="s">
+        <v>98</v>
+      </c>
       <c r="B106" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D106" s="18">
         <v>2</v>
       </c>
-      <c r="E106" s="15">
-        <v>0.2</v>
+      <c r="E106" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G106">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="19"/>
+      <c r="A107" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="B107" s="19" t="s">
         <v>87</v>
       </c>
@@ -3282,10 +3284,10 @@
         <v>2</v>
       </c>
       <c r="E107" s="15">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G107">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3300,10 +3302,10 @@
         <v>2</v>
       </c>
       <c r="E108" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G108">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3318,52 +3320,51 @@
         <v>2</v>
       </c>
       <c r="E109" s="15">
-        <v>1.69</v>
+        <v>0.5</v>
       </c>
       <c r="G109">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="19" t="s">
-        <v>56</v>
-      </c>
+      <c r="A110" s="19"/>
       <c r="B110" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D110" s="18">
         <v>2</v>
       </c>
       <c r="E110" s="15">
-        <v>0</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G110">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="19" t="s">
-        <v>102</v>
-      </c>
+      <c r="A111" s="19"/>
       <c r="B111" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D111" s="18">
         <v>2</v>
       </c>
       <c r="E111" s="15">
-        <v>0</v>
+        <v>1.69</v>
+      </c>
+      <c r="G111">
+        <v>85</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="19" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="B112" s="19" t="s">
         <v>87</v>
@@ -3375,11 +3376,16 @@
         <v>2</v>
       </c>
       <c r="E112" s="15">
-        <v>0.02</v>
+        <v>0</v>
+      </c>
+      <c r="G112">
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="19"/>
+      <c r="A113" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="B113" s="19" t="s">
         <v>87</v>
       </c>
@@ -3390,11 +3396,13 @@
         <v>2</v>
       </c>
       <c r="E113" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="19"/>
+      <c r="A114" s="19" t="s">
+        <v>103</v>
+      </c>
       <c r="B114" s="19" t="s">
         <v>87</v>
       </c>
@@ -3405,20 +3413,38 @@
         <v>2</v>
       </c>
       <c r="E114" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="19"/>
+      <c r="B115" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D115" s="18">
+        <v>2</v>
+      </c>
+      <c r="E115" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="20"/>
-      <c r="B115" s="20"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="22"/>
-    </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="20"/>
-      <c r="B116" s="20"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="22"/>
+      <c r="A116" s="19"/>
+      <c r="B116" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D116" s="18">
+        <v>2</v>
+      </c>
+      <c r="E116" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="20"/>
@@ -4070,11 +4096,13 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="20"/>
+      <c r="B225" s="20"/>
       <c r="C225" s="21"/>
       <c r="D225" s="22"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="20"/>
+      <c r="B226" s="20"/>
       <c r="C226" s="21"/>
       <c r="D226" s="22"/>
     </row>
@@ -4117,6 +4145,16 @@
       <c r="A234" s="20"/>
       <c r="C234" s="21"/>
       <c r="D234" s="22"/>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="20"/>
+      <c r="C235" s="21"/>
+      <c r="D235" s="22"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="20"/>
+      <c r="C236" s="21"/>
+      <c r="D236" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4141,10 +4179,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{FCAB33B4-E22D-416A-9EE8-1B6629F4B7A9}">
       <formula1>"angiosperm, gymnosperm"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E87" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E89" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E88 E83 E85:E86" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E90 E85 E87:E88" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4170,7 +4208,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{793E17DF-C558-4DAF-B608-9E20297CD619}">
       <formula1>"annual, perennial evergreen, perennial deciduous"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E91 E104" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E93 E106" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E20" xr:uid="{DC451139-D175-47A3-922A-D7E1D89FD320}">
@@ -4201,10 +4239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
-  <dimension ref="A1:N234"/>
+  <dimension ref="A1:N236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5072,7 +5110,7 @@
         <v>40</v>
       </c>
       <c r="J49">
-        <f>(E44+E45)/E74*E70</f>
+        <f>(E44+E45)/E75*E70</f>
         <v>0.52222222222222237</v>
       </c>
       <c r="K49">
@@ -5080,7 +5118,7 @@
         <v>-3.2821446515036072</v>
       </c>
       <c r="M49">
-        <f>E70/E75</f>
+        <f>E70/E76</f>
         <v>138.2930051648863</v>
       </c>
       <c r="N49">
@@ -5403,7 +5441,7 @@
         <v>18</v>
       </c>
       <c r="I68">
-        <f>E70/E75</f>
+        <f>E70/E76</f>
         <v>138.2930051648863</v>
       </c>
     </row>
@@ -5461,398 +5499,388 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>110</v>
+        <v>178</v>
       </c>
       <c r="D72" s="18"/>
-      <c r="E72" s="15">
-        <v>0.33</v>
-      </c>
+      <c r="E72" s="15"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B73" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D73" s="18"/>
       <c r="E73" s="15">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B74" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D74" s="18"/>
       <c r="E74" s="15">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" s="18"/>
+      <c r="E75" s="15">
         <f>E70/10</f>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="K74" t="e">
+      <c r="K75" t="e">
         <f>(K67-K68)/K68</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M74" t="e">
+      <c r="M75" t="e">
         <f>(M68-M67)/M68</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B75" s="19" t="s">
+      <c r="B76" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C75" s="17" t="s">
+      <c r="C76" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="27">
+      <c r="D76" s="18"/>
+      <c r="E76" s="27">
         <f>SQRT(0.231/100/100*4/PI())</f>
         <v>5.423267786434878E-3</v>
       </c>
-      <c r="G75">
+      <c r="G76">
         <v>49</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B76" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D76" s="18"/>
-      <c r="E76" s="15">
-        <v>0.02</v>
-      </c>
-      <c r="G76">
-        <v>51</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>125</v>
+        <v>180</v>
       </c>
       <c r="D77" s="18"/>
-      <c r="E77" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="G77">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E77" s="27"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D78" s="18"/>
       <c r="E78" s="15">
-        <v>7.4000000000000003E-3</v>
+        <v>0.02</v>
+      </c>
+      <c r="G78">
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C79" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D79" s="19"/>
+      <c r="C79" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D79" s="18"/>
       <c r="E79" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F79" t="s">
-        <v>115</v>
+        <v>0.01</v>
       </c>
       <c r="G79">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="18"/>
+      <c r="E80" s="15">
+        <v>7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D81" s="19"/>
+      <c r="E81" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F81" t="s">
+        <v>115</v>
+      </c>
+      <c r="G81">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="D80" s="19"/>
-      <c r="E80" s="15">
-        <v>4</v>
-      </c>
-      <c r="F80" s="19" t="s">
+      <c r="D82" s="19"/>
+      <c r="E82" s="15">
+        <v>2</v>
+      </c>
+      <c r="F82" s="19" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+    <row r="83" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="8"/>
-      <c r="G81">
+      <c r="B83" s="5"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="8"/>
+      <c r="G83">
         <v>54</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+    <row r="84" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D82" s="18"/>
-      <c r="E82" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="G82">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="B83" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D83" s="18"/>
-      <c r="E83" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G83">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="19" t="s">
-        <v>114</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>86</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D84" s="18"/>
       <c r="E84" s="15">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
       <c r="G84">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="7"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="8" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B85" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D85" s="18"/>
+      <c r="E85" s="15">
+        <v>0.5</v>
       </c>
       <c r="G85">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="D86" s="18"/>
       <c r="E86" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="G86">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G87">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D88" s="18"/>
+      <c r="E88" s="15">
         <v>0.01</v>
       </c>
-      <c r="G86">
+      <c r="G88">
         <v>59</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="19" t="s">
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B87" s="19" t="s">
+      <c r="B89" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="C89" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D87" s="18"/>
-      <c r="E87" s="15">
+      <c r="D89" s="18"/>
+      <c r="E89" s="15">
         <v>365</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F89" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="5" t="s">
+    <row r="90" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="8"/>
-      <c r="G88">
+      <c r="B90" s="5"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="8"/>
+      <c r="G90">
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="19" t="s">
+    <row r="91" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="B89" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D89" s="18">
-        <v>1</v>
-      </c>
-      <c r="E89" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G89">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D90" s="18">
-        <v>1</v>
-      </c>
-      <c r="E90" s="15">
-        <v>207</v>
-      </c>
-      <c r="G90">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="19" t="s">
-        <v>95</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D91" s="18">
         <v>1</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="G91">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B92" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D92" s="18">
         <v>1</v>
       </c>
       <c r="E92" s="15">
-        <v>30</v>
+        <v>207</v>
       </c>
       <c r="G92">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="19"/>
+      <c r="A93" s="19" t="s">
+        <v>95</v>
+      </c>
       <c r="B93" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D93" s="18">
         <v>1</v>
       </c>
-      <c r="E93" s="15">
-        <v>40</v>
+      <c r="E93" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G93">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="19"/>
+      <c r="A94" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="B94" s="19" t="s">
         <v>87</v>
       </c>
@@ -5863,10 +5891,10 @@
         <v>1</v>
       </c>
       <c r="E94" s="15">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G94">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -5881,10 +5909,10 @@
         <v>1</v>
       </c>
       <c r="E95" s="15">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="G95">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -5898,29 +5926,29 @@
       <c r="D96" s="18">
         <v>1</v>
       </c>
-      <c r="E96" s="15"/>
+      <c r="E96" s="15">
+        <v>50</v>
+      </c>
       <c r="G96">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="19" t="s">
-        <v>52</v>
-      </c>
+      <c r="A97" s="19"/>
       <c r="B97" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D97" s="18">
         <v>1</v>
       </c>
       <c r="E97" s="15">
-        <v>0.01</v>
+        <v>55</v>
       </c>
       <c r="G97">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -5929,20 +5957,20 @@
         <v>87</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D98" s="18">
         <v>1</v>
       </c>
-      <c r="E98" s="15">
-        <v>0.25</v>
-      </c>
+      <c r="E98" s="15"/>
       <c r="G98">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="19"/>
+      <c r="A99" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="B99" s="19" t="s">
         <v>87</v>
       </c>
@@ -5953,10 +5981,10 @@
         <v>1</v>
       </c>
       <c r="E99" s="15">
-        <v>0.67</v>
+        <v>0.01</v>
       </c>
       <c r="G99">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -5971,10 +5999,10 @@
         <v>1</v>
       </c>
       <c r="E100" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="F100" t="s">
-        <v>100</v>
+        <v>0.25</v>
+      </c>
+      <c r="G100">
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -5988,111 +6016,111 @@
       <c r="D101" s="18">
         <v>1</v>
       </c>
-      <c r="E101" s="15"/>
+      <c r="E101" s="15">
+        <v>0.67</v>
+      </c>
       <c r="G101">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="19" t="s">
-        <v>53</v>
-      </c>
+      <c r="A102" s="19"/>
       <c r="B102" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D102" s="18">
-        <v>2</v>
-      </c>
-      <c r="E102" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G102">
-        <v>78</v>
+        <v>1</v>
+      </c>
+      <c r="E102" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F102" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="19" t="s">
-        <v>54</v>
-      </c>
+      <c r="A103" s="19"/>
       <c r="B103" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D103" s="18">
-        <v>2</v>
-      </c>
-      <c r="E103" s="15">
-        <v>365</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E103" s="15"/>
       <c r="G103">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="19" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="B104" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D104" s="18">
         <v>2</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="G104">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B105" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D105" s="18">
         <v>2</v>
       </c>
       <c r="E105" s="15">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="G105">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="19"/>
+      <c r="A106" s="19" t="s">
+        <v>98</v>
+      </c>
       <c r="B106" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D106" s="18">
         <v>2</v>
       </c>
-      <c r="E106" s="15">
-        <v>0.5</v>
+      <c r="E106" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="G106">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="19"/>
+      <c r="A107" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="B107" s="19" t="s">
         <v>87</v>
       </c>
@@ -6103,10 +6131,10 @@
         <v>2</v>
       </c>
       <c r="E107" s="15">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G107">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -6121,10 +6149,10 @@
         <v>2</v>
       </c>
       <c r="E108" s="15">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="G108">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -6139,30 +6167,28 @@
         <v>2</v>
       </c>
       <c r="E109" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="G109">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="19" t="s">
-        <v>56</v>
-      </c>
+      <c r="A110" s="19"/>
       <c r="B110" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D110" s="18">
         <v>2</v>
       </c>
       <c r="E110" s="15">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="G110">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -6171,17 +6197,22 @@
         <v>87</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D111" s="18">
         <v>2</v>
       </c>
       <c r="E111" s="15">
-        <v>0</v>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G111">
+        <v>85</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="19"/>
+      <c r="A112" s="19" t="s">
+        <v>56</v>
+      </c>
       <c r="B112" s="19" t="s">
         <v>87</v>
       </c>
@@ -6192,7 +6223,10 @@
         <v>2</v>
       </c>
       <c r="E112" s="15">
-        <v>0.3</v>
+        <v>0</v>
+      </c>
+      <c r="G112">
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -6207,7 +6241,7 @@
         <v>2</v>
       </c>
       <c r="E113" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -6222,20 +6256,38 @@
         <v>2</v>
       </c>
       <c r="E114" s="15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="19"/>
+      <c r="B115" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D115" s="18">
+        <v>2</v>
+      </c>
+      <c r="E115" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="20"/>
-      <c r="B115" s="20"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="22"/>
-    </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="20"/>
-      <c r="B116" s="20"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="22"/>
+      <c r="A116" s="19"/>
+      <c r="B116" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D116" s="18">
+        <v>2</v>
+      </c>
+      <c r="E116" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="20"/>
@@ -6945,8 +6997,23 @@
       <c r="C234" s="21"/>
       <c r="D234" s="22"/>
     </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="20"/>
+      <c r="B235" s="20"/>
+      <c r="C235" s="21"/>
+      <c r="D235" s="22"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="20"/>
+      <c r="B236" s="20"/>
+      <c r="C236" s="21"/>
+      <c r="D236" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A47:A50"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="A43:A46"/>
@@ -6954,9 +7021,6 @@
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A59:A62"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A47:A50"/>
   </mergeCells>
   <dataValidations count="18">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E36 E19" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
@@ -6969,11 +7033,11 @@
       <formula1>1</formula1>
       <formula2>366</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E88 E83 E85:E86" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E90 E85 E87:E88" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E87" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E89" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{9966BE53-3AF7-47D9-9DC3-79C6924CF42E}">
@@ -6997,7 +7061,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9" xr:uid="{82D88EBD-3D9A-4158-A9B3-F883994282C6}">
       <formula1>"climbing,columnar,conical,decumbent,erect,irregular,oval,prostrate,rounded,semi_erect,vase"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E91 E104" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E93 E106" xr:uid="{3B070726-5ED6-4F50-8EA9-9C057DD1E6C1}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E20 E27" xr:uid="{CC49B6F4-DDA3-41C3-9192-398A844CBA5C}">

</xml_diff>